<commit_message>
save recordingDate not dateTime to CCD
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="301">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -305,13 +305,10 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
-    <t xml:space="preserve">recordingDateTime</t>
+    <t xml:space="preserve">recordingDate</t>
   </si>
   <si>
     <t xml:space="preserve">Recording Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DateTime</t>
   </si>
   <si>
     <t xml:space="preserve">recordingTimeOfDay</t>
@@ -1022,7 +1019,7 @@
     <t xml:space="preserve">BannerUrl</t>
   </si>
   <si>
-    <t xml:space="preserve">true</t>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">Hearing Audio File Search and Retreive</t>
@@ -2348,7 +2345,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -2375,31 +2372,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>208</v>
-      </c>
       <c r="I2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>174</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -2426,28 +2423,28 @@
         <v>19</v>
       </c>
       <c r="D3" s="91" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
-        <v>184</v>
-      </c>
       <c r="F3" s="91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" s="90" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="I3" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="I3" s="90" t="s">
-        <v>211</v>
-      </c>
       <c r="J3" s="90" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K3" s="90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2469,7 +2466,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2491,7 +2488,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="12" t="s">
@@ -2522,31 +2519,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>220</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2560,31 +2557,31 @@
         <v>49</v>
       </c>
       <c r="D3" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="H3" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="H3" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="L3" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>110</v>
       </c>
       <c r="M3" s="61"/>
       <c r="N3" s="61"/>
@@ -2599,10 +2596,10 @@
       </c>
       <c r="D4" s="62"/>
       <c r="E4" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F4" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G4" s="62" t="n">
         <v>1</v>
@@ -2627,10 +2624,10 @@
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G5" s="62" t="n">
         <v>1</v>
@@ -2655,10 +2652,10 @@
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F6" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F6" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G6" s="62" t="n">
         <v>1</v>
@@ -2683,16 +2680,16 @@
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F7" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G7" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="62" t="n">
         <v>5</v>
@@ -2711,16 +2708,16 @@
       </c>
       <c r="D8" s="62"/>
       <c r="E8" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G8" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="62" t="n">
         <v>6</v>
@@ -2739,16 +2736,16 @@
       </c>
       <c r="D9" s="62"/>
       <c r="E9" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="F9" s="93" t="s">
         <v>228</v>
-      </c>
-      <c r="F9" s="93" t="s">
-        <v>229</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I9" s="62" t="n">
         <v>7</v>
@@ -2767,16 +2764,16 @@
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="92" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="62" t="n">
         <v>2</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I10" s="62" t="n">
         <v>1</v>
@@ -2831,7 +2828,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="95" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B1" s="96" t="s">
         <v>8</v>
@@ -2866,22 +2863,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="102" t="s">
         <v>232</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="G2" s="103" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="G2" s="103" t="s">
-        <v>206</v>
-      </c>
-      <c r="H2" s="103" t="s">
+      <c r="I2" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="J2" s="102" t="s">
         <v>235</v>
-      </c>
-      <c r="J2" s="102" t="s">
-        <v>236</v>
       </c>
       <c r="K2" s="103"/>
       <c r="L2" s="105"/>
@@ -2904,22 +2901,22 @@
         <v>50</v>
       </c>
       <c r="F3" s="107" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="107" t="s">
         <v>237</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="H3" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="I3" s="108" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="I3" s="108" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="108" t="s">
+      <c r="K3" s="108" t="s">
         <v>240</v>
-      </c>
-      <c r="K3" s="108" t="s">
-        <v>241</v>
       </c>
       <c r="L3" s="108"/>
       <c r="M3" s="109"/>
@@ -3014,7 +3011,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3034,7 +3031,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="111" t="s">
         <v>8</v>
@@ -3063,25 +3060,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,25 +3092,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="115" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>64</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3125,11 +3122,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="74" t="n">
@@ -3169,11 +3166,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="50"/>
       <c r="H6" s="74" t="n">
@@ -3191,11 +3188,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="74" t="n">
@@ -3213,11 +3210,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="74" t="n">
@@ -3302,7 +3299,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3322,7 +3319,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3350,22 +3347,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="117" t="s">
         <v>249</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="117" t="s">
-        <v>250</v>
       </c>
       <c r="J2" s="118"/>
       <c r="K2" s="119"/>
@@ -3383,10 +3380,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="120" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="90" t="s">
         <v>64</v>
@@ -3395,10 +3392,10 @@
         <v>50</v>
       </c>
       <c r="H3" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="121" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J3" s="122"/>
       <c r="K3" s="123"/>
@@ -3414,11 +3411,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -3458,11 +3455,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -3480,11 +3477,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -3502,11 +3499,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="74" t="n">
         <v>6</v>
@@ -3598,7 +3595,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="126" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
         <v>8</v>
@@ -3619,16 +3616,16 @@
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="128" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="128" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="128" t="s">
-        <v>247</v>
-      </c>
-      <c r="E2" s="128" t="s">
+      <c r="F2" s="89" t="s">
         <v>253</v>
-      </c>
-      <c r="F2" s="89" t="s">
-        <v>254</v>
       </c>
       <c r="G2" s="89"/>
       <c r="H2" s="89"/>
@@ -3645,7 +3642,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="130" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="129" t="s">
         <v>64</v>
@@ -3654,13 +3651,13 @@
         <v>50</v>
       </c>
       <c r="G3" s="129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H3" s="129" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="129" t="s">
         <v>255</v>
-      </c>
-      <c r="I3" s="129" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3682,7 +3679,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3701,7 +3698,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="132" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="133" t="s">
         <v>8</v>
@@ -3730,25 +3727,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3762,25 +3759,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
       <c r="G3" s="90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="90" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J3" s="90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3792,11 +3789,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="74" t="n">
@@ -3836,11 +3833,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="74" t="n">
@@ -3858,11 +3855,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="74" t="n">
@@ -3880,11 +3877,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="74" t="n">
@@ -3924,11 +3921,11 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="74" t="n">
@@ -3957,7 +3954,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3976,7 +3973,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4004,22 +4001,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4033,10 +4030,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="120" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="90" t="s">
         <v>64</v>
@@ -4045,10 +4042,10 @@
         <v>50</v>
       </c>
       <c r="H3" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I3" s="90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J3" s="123"/>
       <c r="K3" s="123"/>
@@ -4064,11 +4061,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -4108,11 +4105,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -4130,11 +4127,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -4152,11 +4149,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="74" t="n">
         <v>6</v>
@@ -4196,11 +4193,11 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G10" s="74" t="n">
         <v>8</v>
@@ -4275,7 +4272,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4298,13 +4295,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
         <v>262</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4315,16 +4312,16 @@
         <v>18</v>
       </c>
       <c r="C3" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="E3" s="79" t="s">
         <v>265</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="F3" s="79" t="s">
         <v>266</v>
-      </c>
-      <c r="F3" s="79" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4333,7 +4330,7 @@
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="138" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="138" t="s">
         <v>23</v>
@@ -4385,7 +4382,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4407,16 +4404,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>270</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4606,7 +4603,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4627,13 +4624,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="34" t="s">
         <v>274</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4647,10 +4644,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4662,10 +4659,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -4701,7 +4698,7 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4718,7 +4715,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="141" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4744,16 +4741,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>280</v>
-      </c>
       <c r="E2" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>274</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>275</v>
       </c>
       <c r="G2" s="128"/>
       <c r="H2" s="128"/>
@@ -4772,13 +4769,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="144" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="144" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="143" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G3" s="89"/>
       <c r="H3" s="89"/>
@@ -4798,10 +4795,10 @@
         <v>71</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -4825,10 +4822,10 @@
         <v>75</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4843,10 +4840,10 @@
         <v>79</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4858,13 +4855,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4876,13 +4873,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4894,13 +4891,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4912,13 +4909,13 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4930,13 +4927,13 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4948,13 +4945,13 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4966,13 +4963,13 @@
         <v>38</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5037,7 +5034,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5059,16 +5056,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="34" t="s">
         <v>274</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>275</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -5087,13 +5084,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="145" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E3" s="145" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5105,13 +5102,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5123,13 +5120,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5141,13 +5138,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5159,13 +5156,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5212,7 +5209,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="147" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B1" s="148" t="s">
         <v>8</v>
@@ -5234,16 +5231,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="152" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>274</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>275</v>
       </c>
       <c r="G2" s="153"/>
       <c r="H2" s="153"/>
@@ -5262,13 +5259,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="145" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E3" s="145" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F3" s="154" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5283,10 +5280,10 @@
         <v>52</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -5320,7 +5317,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -5338,7 +5335,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5357,19 +5354,19 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,16 +5380,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="76" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G3" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5404,16 +5401,16 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5425,16 +5422,16 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5446,16 +5443,16 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -5478,7 +5475,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5492,7 +5489,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="155" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B1" s="156"/>
       <c r="C1" s="156"/>
@@ -5500,44 +5497,44 @@
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="158" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="158" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="158" t="s">
+      <c r="C2" s="158" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="158" t="s">
+      <c r="D2" s="158" t="s">
         <v>292</v>
-      </c>
-      <c r="D2" s="158" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="159" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" s="159" t="s">
         <v>294</v>
       </c>
-      <c r="B3" s="159" t="s">
+      <c r="C3" s="159" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="D3" s="159" t="s">
         <v>296</v>
-      </c>
-      <c r="D3" s="159" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="160" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="161" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="C4" s="161" t="s">
         <v>299</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="D4" s="25" t="s">
         <v>300</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5875,8 +5872,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6345,7 +6342,7 @@
       </c>
       <c r="F6" s="62"/>
       <c r="G6" s="62" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="H6" s="62"/>
       <c r="I6" s="62"/>
@@ -6500,13 +6497,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="F7" s="62" t="s">
         <v>83</v>
-      </c>
-      <c r="F7" s="62" t="s">
-        <v>84</v>
       </c>
       <c r="G7" s="51" t="s">
         <v>78</v>
@@ -6664,10 +6661,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="52" t="s">
         <v>85</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>86</v>
       </c>
       <c r="F8" s="62"/>
       <c r="G8" s="51" t="s">
@@ -6826,10 +6823,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="52" t="s">
         <v>87</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>88</v>
       </c>
       <c r="F9" s="62"/>
       <c r="G9" s="51" t="s">
@@ -6988,10 +6985,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="52" t="s">
         <v>89</v>
-      </c>
-      <c r="E10" s="52" t="s">
-        <v>90</v>
       </c>
       <c r="F10" s="62"/>
       <c r="G10" s="51" t="s">
@@ -7150,10 +7147,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="52" t="s">
         <v>91</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>92</v>
       </c>
       <c r="F11" s="62"/>
       <c r="G11" s="51" t="s">
@@ -7312,17 +7309,17 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="52" t="s">
         <v>93</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>94</v>
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="52" t="s">
         <v>95</v>
-      </c>
-      <c r="H12" s="52" t="s">
-        <v>96</v>
       </c>
       <c r="I12" s="62"/>
       <c r="J12" s="51" t="s">
@@ -7476,10 +7473,10 @@
         <v>38</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>97</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>98</v>
       </c>
       <c r="F13" s="62"/>
       <c r="G13" s="51" t="s">
@@ -9476,7 +9473,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -9507,10 +9504,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>59</v>
@@ -9519,16 +9516,16 @@
         <v>60</v>
       </c>
       <c r="G2" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="I2" s="34" t="s">
         <v>61</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>33</v>
@@ -9540,10 +9537,10 @@
         <v>63</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="69" t="s">
         <v>105</v>
-      </c>
-      <c r="O2" s="69" t="s">
-        <v>106</v>
       </c>
       <c r="P2" s="70"/>
       <c r="Q2" s="47"/>
@@ -9560,7 +9557,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>66</v>
@@ -9569,10 +9566,10 @@
         <v>67</v>
       </c>
       <c r="G3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>108</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>109</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>68</v>
@@ -9593,7 +9590,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P3" s="73"/>
       <c r="Q3" s="61"/>
@@ -9605,17 +9602,17 @@
       </c>
       <c r="B4" s="62"/>
       <c r="C4" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>111</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>112</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="62"/>
       <c r="I4" s="74"/>
@@ -9634,22 +9631,22 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="52" t="s">
         <v>114</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>115</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K5" s="51" t="s">
         <v>41</v>
@@ -9905,22 +9902,22 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" s="62"/>
       <c r="I6" s="62"/>
       <c r="J6" s="52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="51" t="s">
         <v>41</v>
@@ -10276,7 +10273,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10298,16 +10295,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="F2" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -10325,10 +10322,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="76" t="s">
         <v>50</v>
@@ -10347,10 +10344,10 @@
         <v>71</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="62" t="n">
         <v>1</v>
@@ -10365,10 +10362,10 @@
         <v>71</v>
       </c>
       <c r="D5" s="77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" s="62" t="n">
         <v>2</v>
@@ -10393,8 +10390,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10424,7 +10421,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10463,55 +10460,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>135</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="M2" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="M2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="N2" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="P2" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10537,43 +10534,43 @@
         <v>50</v>
       </c>
       <c r="H3" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="79" t="s">
         <v>142</v>
-      </c>
-      <c r="I3" s="79" t="s">
-        <v>143</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K3" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="M3" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="P3" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="R3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="S3" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="S3" s="76" t="s">
+      <c r="T3" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="76" t="s">
+      <c r="U3" s="76" t="s">
         <v>152</v>
-      </c>
-      <c r="U3" s="76" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10585,13 +10582,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>155</v>
-      </c>
-      <c r="F4" s="52" t="s">
-        <v>156</v>
       </c>
       <c r="G4" s="50" t="n">
         <v>1</v>
@@ -10609,9 +10606,9 @@
       <c r="N4" s="50"/>
       <c r="O4" s="50"/>
       <c r="P4" s="50"/>
-      <c r="R4" s="50"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T4" s="50"/>
       <c r="U4" s="50"/>
@@ -10625,13 +10622,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="F5" s="51" t="s">
         <v>159</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>160</v>
       </c>
       <c r="G5" s="50" t="n">
         <v>2</v>
@@ -10651,9 +10648,9 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
-      <c r="R5" s="50"/>
+      <c r="R5" s="80"/>
       <c r="S5" s="80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
@@ -10667,13 +10664,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="F6" s="51" t="s">
         <v>162</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>163</v>
       </c>
       <c r="G6" s="50" t="n">
         <v>3</v>
@@ -10693,9 +10690,9 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="R6" s="50"/>
+      <c r="R6" s="80"/>
       <c r="S6" s="80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T6" s="50"/>
       <c r="U6" s="50"/>
@@ -10709,13 +10706,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="F7" s="25" t="s">
         <v>165</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>166</v>
       </c>
       <c r="G7" s="50" t="n">
         <v>4</v>
@@ -10736,12 +10733,14 @@
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
       <c r="O7" s="82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P7" s="50"/>
-      <c r="R7" s="50"/>
+      <c r="R7" s="80" t="s">
+        <v>156</v>
+      </c>
       <c r="S7" s="80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
@@ -10768,7 +10767,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10786,7 +10785,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="47.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="47.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="11" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="28.3"/>
@@ -10797,7 +10796,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10836,55 +10835,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="O2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="R2" s="16" t="s">
-        <v>182</v>
-      </c>
       <c r="S2" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="T2" s="34" t="s">
         <v>136</v>
-      </c>
-      <c r="T2" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
@@ -10911,55 +10910,55 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="F3" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="G3" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="H3" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="K3" s="22" t="s">
+      <c r="L3" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="M3" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="O3" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="83" t="s">
         <v>192</v>
       </c>
-      <c r="O3" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="83" t="s">
+      <c r="Q3" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="S3" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="T3" s="21" t="s">
         <v>196</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10971,7 +10970,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>71</v>
@@ -10982,11 +10981,11 @@
         <v>1</v>
       </c>
       <c r="I4" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J4" s="62"/>
       <c r="K4" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L4" s="51"/>
       <c r="M4" s="62" t="n">
@@ -11009,7 +11008,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="52" t="s">
         <v>75</v>
@@ -11020,11 +11019,11 @@
         <v>1</v>
       </c>
       <c r="I5" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J5" s="62"/>
       <c r="K5" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L5" s="51"/>
       <c r="M5" s="62" t="n">
@@ -11047,22 +11046,24 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+      <c r="G6" s="51" t="s">
+        <v>3</v>
+      </c>
       <c r="H6" s="74" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J6" s="62"/>
       <c r="K6" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L6" s="51"/>
       <c r="M6" s="62" t="n">
@@ -11085,10 +11086,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -11096,11 +11097,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L7" s="51"/>
       <c r="M7" s="62" t="n">
@@ -11123,10 +11124,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -11134,11 +11135,11 @@
         <v>1</v>
       </c>
       <c r="I8" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L8" s="51"/>
       <c r="M8" s="62" t="n">
@@ -11161,10 +11162,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -11172,11 +11173,11 @@
         <v>1</v>
       </c>
       <c r="I9" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J9" s="62"/>
       <c r="K9" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L9" s="51"/>
       <c r="M9" s="62" t="n">
@@ -11199,10 +11200,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -11210,11 +11211,11 @@
         <v>1</v>
       </c>
       <c r="I10" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J10" s="62"/>
       <c r="K10" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L10" s="51"/>
       <c r="M10" s="62" t="n">
@@ -11237,10 +11238,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -11248,11 +11249,11 @@
         <v>1</v>
       </c>
       <c r="I11" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J11" s="62"/>
       <c r="K11" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L11" s="51"/>
       <c r="M11" s="62" t="n">
@@ -11275,7 +11276,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="52" t="s">
         <v>79</v>
@@ -11286,11 +11287,11 @@
         <v>1</v>
       </c>
       <c r="I12" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J12" s="62"/>
       <c r="K12" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L12" s="51"/>
       <c r="M12" s="62" t="n">
@@ -11313,7 +11314,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="52" t="s">
         <v>71</v>
@@ -11324,11 +11325,11 @@
         <v>1</v>
       </c>
       <c r="I13" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J13" s="62"/>
       <c r="K13" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L13" s="51"/>
       <c r="M13" s="62" t="n">
@@ -11351,7 +11352,7 @@
         <v>38</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="52" t="s">
         <v>75</v>
@@ -11362,11 +11363,11 @@
         <v>1</v>
       </c>
       <c r="I14" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J14" s="62"/>
       <c r="K14" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L14" s="51"/>
       <c r="M14" s="62" t="n">
@@ -11389,7 +11390,7 @@
         <v>38</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>79</v>
@@ -11400,11 +11401,11 @@
         <v>1</v>
       </c>
       <c r="I15" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J15" s="62"/>
       <c r="K15" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L15" s="51"/>
       <c r="M15" s="62" t="n">
@@ -11427,10 +11428,10 @@
         <v>38</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -11438,11 +11439,11 @@
         <v>1</v>
       </c>
       <c r="I16" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J16" s="62"/>
       <c r="K16" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L16" s="51"/>
       <c r="M16" s="62" t="n">
@@ -11465,10 +11466,10 @@
         <v>38</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -11476,11 +11477,11 @@
         <v>1</v>
       </c>
       <c r="I17" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J17" s="62"/>
       <c r="K17" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L17" s="51"/>
       <c r="M17" s="62" t="n">
@@ -11503,10 +11504,10 @@
         <v>38</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -11514,11 +11515,11 @@
         <v>1</v>
       </c>
       <c r="I18" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L18" s="51"/>
       <c r="M18" s="62" t="n">
@@ -11541,10 +11542,10 @@
         <v>38</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -11552,11 +11553,11 @@
         <v>1</v>
       </c>
       <c r="I19" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19" s="62"/>
       <c r="K19" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L19" s="51"/>
       <c r="M19" s="62" t="n">
@@ -11579,10 +11580,10 @@
         <v>38</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -11590,11 +11591,11 @@
         <v>1</v>
       </c>
       <c r="I20" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J20" s="62"/>
       <c r="K20" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L20" s="51"/>
       <c r="M20" s="62" t="n">
@@ -11617,10 +11618,10 @@
         <v>38</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -11628,11 +11629,11 @@
         <v>1</v>
       </c>
       <c r="I21" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J21" s="62"/>
       <c r="K21" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L21" s="51"/>
       <c r="M21" s="62" t="n">
@@ -11655,10 +11656,10 @@
         <v>38</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -11666,11 +11667,11 @@
         <v>1</v>
       </c>
       <c r="I22" s="84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J22" s="62"/>
       <c r="K22" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L22" s="51"/>
       <c r="M22" s="62" t="n">
@@ -11693,10 +11694,10 @@
         <v>38</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -11704,11 +11705,11 @@
         <v>1</v>
       </c>
       <c r="I23" s="86" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J23" s="62"/>
       <c r="K23" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L23" s="51"/>
       <c r="M23" s="62" t="n">

</xml_diff>

<commit_message>
rename recordingReference to caseReference in CCD
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -338,10 +338,10 @@
     <t xml:space="preserve">Court Location Code</t>
   </si>
   <si>
-    <t xml:space="preserve">recordingReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recording Reference</t>
+    <t xml:space="preserve">caseReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Reference</t>
   </si>
   <si>
     <t xml:space="preserve">recordingFiles</t>
@@ -1043,7 +1043,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1209,6 +1209,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1460,7 +1465,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1473,7 +1478,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="167">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1734,6 +1739,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="24" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1794,7 +1803,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1802,7 +1811,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1818,6 +1827,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1918,10 +1931,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1930,15 +1939,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1946,7 +1959,51 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1954,59 +2011,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2014,11 +2019,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2030,7 +2043,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2038,7 +2051,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2118,7 +2131,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2126,11 +2139,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2413,37 +2426,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="93" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="92" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="90" t="s">
+      <c r="K3" s="92" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2466,7 +2479,7 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2595,10 +2608,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2623,10 +2636,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2651,10 +2664,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="93" t="s">
+      <c r="F6" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2679,10 +2692,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2707,10 +2720,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2735,16 +2748,16 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="94" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="95" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="87" t="s">
         <v>90</v>
       </c>
       <c r="I9" s="62" t="n">
@@ -2763,10 +2776,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="92" t="s">
+      <c r="E10" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="95" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2783,10 +2796,11 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="89"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="88"/>
-    </row>
+      <c r="H11" s="90"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2813,184 +2827,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="94" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="94" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="94" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="94" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="94" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="94" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="94" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="94" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="94" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="96" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="96" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="96" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="96" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="96" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="96" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="104" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="104" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="105" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="H2" s="105" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="102" t="s">
+      <c r="J2" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="107"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="107" t="s">
+      <c r="F3" s="109" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="G3" s="109" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="H3" s="110" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="I3" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="108" t="s">
+      <c r="J3" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="109"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="111"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="112"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="112"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3011,7 +3025,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3033,20 +3047,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="115" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3088,10 +3102,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="117" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3117,11 +3131,11 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="87" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="51"/>
@@ -3129,7 +3143,7 @@
         <v>91</v>
       </c>
       <c r="G4" s="50"/>
-      <c r="H4" s="74" t="n">
+      <c r="H4" s="75" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="50"/>
@@ -3151,7 +3165,7 @@
         <v>76</v>
       </c>
       <c r="G5" s="50"/>
-      <c r="H5" s="74" t="n">
+      <c r="H5" s="75" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="50"/>
@@ -3173,7 +3187,7 @@
         <v>87</v>
       </c>
       <c r="G6" s="50"/>
-      <c r="H6" s="74" t="n">
+      <c r="H6" s="75" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="50"/>
@@ -3195,7 +3209,7 @@
         <v>89</v>
       </c>
       <c r="G7" s="50"/>
-      <c r="H7" s="74" t="n">
+      <c r="H7" s="75" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="50"/>
@@ -3217,7 +3231,7 @@
         <v>85</v>
       </c>
       <c r="G8" s="50"/>
-      <c r="H8" s="74" t="n">
+      <c r="H8" s="75" t="n">
         <v>6</v>
       </c>
       <c r="I8" s="50"/>
@@ -3239,44 +3253,44 @@
         <v>80</v>
       </c>
       <c r="G9" s="62"/>
-      <c r="H9" s="74" t="n">
+      <c r="H9" s="75" t="n">
         <v>7</v>
       </c>
       <c r="I9" s="62"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="65"/>
+      <c r="E10" s="66"/>
     </row>
     <row r="11" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="65"/>
+      <c r="E11" s="66"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="65"/>
+      <c r="E12" s="66"/>
     </row>
     <row r="13" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="65"/>
+      <c r="E13" s="66"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="65"/>
+      <c r="E14" s="66"/>
     </row>
     <row r="15" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="65"/>
+      <c r="E15" s="66"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="65"/>
+      <c r="E16" s="66"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="65"/>
+      <c r="E17" s="66"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="65"/>
+      <c r="E18" s="66"/>
     </row>
     <row r="19" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="65"/>
+      <c r="E19" s="66"/>
     </row>
     <row r="20" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="65"/>
+      <c r="E20" s="66"/>
     </row>
     <row r="21" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3299,7 +3313,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3334,7 +3348,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -3361,48 +3375,48 @@
       <c r="H2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="117" t="s">
+      <c r="I2" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="121" t="s">
+      <c r="I3" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="122"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-    </row>
-    <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J3" s="124"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+    </row>
+    <row r="4" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3410,25 +3424,25 @@
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="87" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="74" t="n">
+      <c r="G4" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-    </row>
-    <row r="5" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+    </row>
+    <row r="5" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -3439,18 +3453,18 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="74" t="n">
+      <c r="G5" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-    </row>
-    <row r="6" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+    </row>
+    <row r="6" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -3461,18 +3475,18 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="74" t="n">
+      <c r="G6" s="75" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-    </row>
-    <row r="7" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+    </row>
+    <row r="7" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -3483,14 +3497,14 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="74" t="n">
+      <c r="G7" s="75" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-    </row>
-    <row r="8" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+    </row>
+    <row r="8" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3505,14 +3519,14 @@
       <c r="F8" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="74" t="n">
+      <c r="G8" s="75" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="124" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="126" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3527,7 +3541,7 @@
       <c r="F9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="74" t="n">
+      <c r="G9" s="75" t="n">
         <v>7</v>
       </c>
       <c r="H9" s="25"/>
@@ -3535,26 +3549,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="87"/>
+      <c r="A10" s="89"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="125"/>
+      <c r="G10" s="127"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="89"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="125"/>
+      <c r="G11" s="127"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="G12" s="125"/>
+      <c r="A12" s="89"/>
+      <c r="G12" s="127"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="G13" s="125"/>
+      <c r="A13" s="89"/>
+      <c r="G13" s="127"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="G14" s="125"/>
+      <c r="A14" s="89"/>
+      <c r="G14" s="127"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3594,7 +3608,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="128" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3603,60 +3617,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="128" t="s">
+      <c r="A2" s="91"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="130" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="130" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="130" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="91" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="130" t="s">
+      <c r="C3" s="132" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="130" t="s">
+      <c r="D3" s="132" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="129" t="s">
+      <c r="E3" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="131" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="131" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3679,41 +3693,41 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="131" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="131" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="133" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="133" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="131" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="131" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="133" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="133" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="133" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="134" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="136" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3749,34 +3763,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="92" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3792,11 +3806,11 @@
         <v>90</v>
       </c>
       <c r="E4" s="52"/>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74" t="n">
+      <c r="G4" s="75"/>
+      <c r="H4" s="75" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="50"/>
@@ -3806,7 +3820,7 @@
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -3817,8 +3831,8 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74" t="n">
+      <c r="G5" s="75"/>
+      <c r="H5" s="75" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="50"/>
@@ -3828,7 +3842,7 @@
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -3839,8 +3853,8 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74" t="n">
+      <c r="G6" s="75"/>
+      <c r="H6" s="75" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="50"/>
@@ -3850,7 +3864,7 @@
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -3861,8 +3875,8 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74" t="n">
+      <c r="G7" s="75"/>
+      <c r="H7" s="75" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="50"/>
@@ -3884,10 +3898,10 @@
         <v>85</v>
       </c>
       <c r="G8" s="25"/>
-      <c r="H8" s="74" t="n">
+      <c r="H8" s="75" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="136"/>
+      <c r="I8" s="138"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3898,7 +3912,7 @@
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="87" t="s">
         <v>79</v>
       </c>
       <c r="E9" s="25"/>
@@ -3906,10 +3920,10 @@
         <v>80</v>
       </c>
       <c r="G9" s="25"/>
-      <c r="H9" s="74" t="n">
+      <c r="H9" s="75" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="136"/>
+      <c r="I9" s="138"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3928,10 +3942,10 @@
         <v>257</v>
       </c>
       <c r="G10" s="25"/>
-      <c r="H10" s="74" t="n">
+      <c r="H10" s="75" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="136"/>
+      <c r="I10" s="138"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3954,7 +3968,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4020,37 +4034,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="122" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="92" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4060,14 +4074,14 @@
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="87" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="74" t="n">
+      <c r="G4" s="75" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="50"/>
@@ -4089,7 +4103,7 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="74" t="n">
+      <c r="G5" s="75" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="50"/>
@@ -4111,7 +4125,7 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="74" t="n">
+      <c r="G6" s="75" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="50"/>
@@ -4133,7 +4147,7 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="74" t="n">
+      <c r="G7" s="75" t="n">
         <v>4</v>
       </c>
       <c r="H7" s="50"/>
@@ -4155,7 +4169,7 @@
       <c r="F8" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="74" t="n">
+      <c r="G8" s="75" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="50"/>
@@ -4177,7 +4191,7 @@
       <c r="F9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="74" t="n">
+      <c r="G9" s="75" t="n">
         <v>7</v>
       </c>
       <c r="H9" s="50"/>
@@ -4199,7 +4213,7 @@
       <c r="F10" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="G10" s="74" t="n">
+      <c r="G10" s="75" t="n">
         <v>8</v>
       </c>
       <c r="H10" s="50"/>
@@ -4207,32 +4221,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="F11" s="137"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="F11" s="139"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="F12" s="137"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="F12" s="139"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
-      <c r="F13" s="137"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="139"/>
+      <c r="F13" s="139"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="F14" s="137"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="139"/>
+      <c r="F14" s="139"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4314,13 +4328,13 @@
       <c r="C3" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="80" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4329,10 +4343,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="140" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="138" t="s">
+      <c r="D4" s="140" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4343,8 +4357,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
-      <c r="C5" s="139"/>
+      <c r="A5" s="89"/>
+      <c r="C5" s="141"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4417,31 +4431,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="140" t="s">
+      <c r="D3" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="92" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="87"/>
+      <c r="A4" s="89"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
+      <c r="A5" s="89"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4654,7 +4668,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4697,8 +4711,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4714,7 +4728,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="143" t="s">
         <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4726,12 +4740,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4752,42 +4766,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="146" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="F3" s="145" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4814,7 +4828,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4832,7 +4846,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4850,7 +4864,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4868,7 +4882,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="116"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4886,7 +4900,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="116"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4904,7 +4918,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="116"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4922,11 +4936,11 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="87" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -4940,7 +4954,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="116"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4958,7 +4972,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="118"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -5080,13 +5094,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="147" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5097,7 +5111,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5115,7 +5129,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5133,7 +5147,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5151,7 +5165,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5197,31 +5211,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="146" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="146" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="146" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="146" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="146" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="146" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="149" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="151" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="150" t="s">
+      <c r="D1" s="152" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5233,7 +5247,7 @@
       <c r="C2" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="152" t="s">
+      <c r="D2" s="154" t="s">
         <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5242,29 +5256,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="155"/>
+      <c r="J2" s="155"/>
+      <c r="K2" s="155"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="147" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="147" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="156" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5370,10 +5384,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="48" t="s">
@@ -5385,10 +5399,10 @@
       <c r="E3" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="77" t="s">
         <v>221</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="77" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5480,73 +5494,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="124" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="124" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="126" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="126" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="126" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="126" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="126" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="157" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="157"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="159"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="160" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="158" t="s">
+      <c r="B2" s="160" t="s">
         <v>290</v>
       </c>
-      <c r="C2" s="158" t="s">
+      <c r="C2" s="160" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="158" t="s">
+      <c r="D2" s="160" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="159" t="s">
+      <c r="B3" s="161" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="C3" s="161" t="s">
         <v>295</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="161" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="160" t="s">
+    <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="162" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="C4" s="163" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="162"/>
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="164"/>
-    </row>
-    <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="164"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="166"/>
+    </row>
+    <row r="6" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5872,8 +5886,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7146,7 +7160,7 @@
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="65" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -7629,13 +7643,13 @@
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="55"/>
       <c r="C14" s="56"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="65"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="66"/>
       <c r="I14" s="53"/>
-      <c r="J14" s="66"/>
+      <c r="J14" s="67"/>
       <c r="K14" s="53"/>
       <c r="L14" s="53"/>
       <c r="M14" s="53"/>
@@ -8021,10 +8035,10 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="67"/>
       <c r="AHE16" s="0"/>
       <c r="AHF16" s="0"/>
       <c r="AHG16" s="0"/>
@@ -8163,9 +8177,9 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="67"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="68"/>
       <c r="AHE17" s="0"/>
       <c r="AHF17" s="0"/>
       <c r="AHG17" s="0"/>
@@ -8304,10 +8318,10 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="67"/>
       <c r="AHE18" s="0"/>
       <c r="AHF18" s="0"/>
       <c r="AHG18" s="0"/>
@@ -8446,8 +8460,8 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="65"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
       <c r="AHE19" s="0"/>
       <c r="AHF19" s="0"/>
       <c r="AHG19" s="0"/>
@@ -8586,8 +8600,8 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
       <c r="AHE20" s="0"/>
       <c r="AHF20" s="0"/>
       <c r="AHG20" s="0"/>
@@ -8726,8 +8740,8 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
       <c r="AHE21" s="0"/>
       <c r="AHF21" s="0"/>
       <c r="AHG21" s="0"/>
@@ -8866,8 +8880,8 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
       <c r="AHE22" s="0"/>
       <c r="AHF22" s="0"/>
       <c r="AHG22" s="0"/>
@@ -9006,8 +9020,8 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
       <c r="AHE23" s="0"/>
       <c r="AHF23" s="0"/>
       <c r="AHG23" s="0"/>
@@ -9146,11 +9160,11 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="53"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="65"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="66"/>
       <c r="AHE24" s="0"/>
       <c r="AHF24" s="0"/>
       <c r="AHG24" s="0"/>
@@ -9289,8 +9303,8 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
       <c r="AHE25" s="0"/>
       <c r="AHF25" s="0"/>
       <c r="AHG25" s="0"/>
@@ -9494,7 +9508,7 @@
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
-      <c r="O1" s="68"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -9539,10 +9553,10 @@
       <c r="N2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="69" t="s">
+      <c r="O2" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="70"/>
+      <c r="P2" s="71"/>
       <c r="Q2" s="47"/>
       <c r="R2" s="47"/>
     </row>
@@ -9553,10 +9567,10 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="72" t="s">
         <v>106</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -9589,10 +9603,10 @@
       <c r="N3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="72" t="s">
+      <c r="O3" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="73"/>
+      <c r="P3" s="74"/>
       <c r="Q3" s="61"/>
       <c r="R3" s="61"/>
     </row>
@@ -9615,7 +9629,7 @@
         <v>112</v>
       </c>
       <c r="H4" s="62"/>
-      <c r="I4" s="74"/>
+      <c r="I4" s="75"/>
       <c r="J4" s="62"/>
       <c r="K4" s="51" t="s">
         <v>41</v>
@@ -10168,75 +10182,75 @@
       <c r="IU6" s="53"/>
     </row>
     <row r="7" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
       <c r="F7" s="53"/>
-      <c r="G7" s="65"/>
+      <c r="G7" s="66"/>
     </row>
     <row r="8" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="53"/>
-      <c r="G8" s="65"/>
-      <c r="I8" s="75"/>
+      <c r="G8" s="66"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="53"/>
-      <c r="G9" s="65"/>
+      <c r="G9" s="66"/>
     </row>
     <row r="10" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="53"/>
-      <c r="G10" s="65"/>
-      <c r="J10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="J10" s="67"/>
     </row>
     <row r="11" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
       <c r="F11" s="53"/>
-      <c r="G11" s="65"/>
-      <c r="I11" s="75"/>
+      <c r="G11" s="66"/>
+      <c r="I11" s="76"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="53"/>
-      <c r="G12" s="65"/>
-      <c r="J12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="J12" s="67"/>
     </row>
     <row r="13" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="65"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="65"/>
-      <c r="J14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="J14" s="67"/>
     </row>
     <row r="15" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="53"/>
-      <c r="G15" s="65"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="53"/>
-      <c r="G16" s="65"/>
+      <c r="G16" s="66"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="53"/>
-      <c r="G17" s="65"/>
+      <c r="G17" s="66"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -10327,7 +10341,7 @@
       <c r="E3" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="77" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="61"/>
@@ -10343,10 +10357,10 @@
       <c r="C4" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="78" t="s">
         <v>126</v>
       </c>
       <c r="F4" s="62" t="n">
@@ -10361,10 +10375,10 @@
       <c r="C5" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="78" t="s">
         <v>127</v>
       </c>
       <c r="F5" s="62" t="n">
@@ -10438,12 +10452,12 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
       <c r="R1" s="15"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
@@ -10533,10 +10547,10 @@
       <c r="G3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="80" t="s">
         <v>142</v>
       </c>
       <c r="J3" s="20" t="s">
@@ -10563,13 +10577,13 @@
       <c r="R3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="S3" s="76" t="s">
+      <c r="S3" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="76" t="s">
+      <c r="T3" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="U3" s="76" t="s">
+      <c r="U3" s="77" t="s">
         <v>152</v>
       </c>
     </row>
@@ -10606,8 +10620,8 @@
       <c r="N4" s="50"/>
       <c r="O4" s="50"/>
       <c r="P4" s="50"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80" t="s">
+      <c r="R4" s="81"/>
+      <c r="S4" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T4" s="50"/>
@@ -10648,8 +10662,8 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="80" t="s">
+      <c r="R5" s="81"/>
+      <c r="S5" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T5" s="50"/>
@@ -10690,8 +10704,8 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80" t="s">
+      <c r="R6" s="81"/>
+      <c r="S6" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T6" s="50"/>
@@ -10726,20 +10740,20 @@
       <c r="J7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="81"/>
+      <c r="K7" s="82"/>
       <c r="L7" s="50" t="n">
         <v>5</v>
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="82" t="s">
+      <c r="O7" s="83" t="s">
         <v>166</v>
       </c>
       <c r="P7" s="50"/>
-      <c r="R7" s="80" t="s">
+      <c r="R7" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="S7" s="80" t="s">
+      <c r="S7" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T7" s="50"/>
@@ -10767,7 +10781,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10945,7 +10959,7 @@
       <c r="O3" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="83" t="s">
+      <c r="P3" s="84" t="s">
         <v>192</v>
       </c>
       <c r="Q3" s="21" t="s">
@@ -10965,7 +10979,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="74"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -10977,14 +10991,14 @@
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
-      <c r="H4" s="74" t="n">
+      <c r="H4" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J4" s="62"/>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L4" s="51"/>
@@ -10995,7 +11009,7 @@
       <c r="O4" s="62"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="51"/>
-      <c r="R4" s="74"/>
+      <c r="R4" s="75"/>
       <c r="S4" s="62"/>
       <c r="T4" s="62"/>
     </row>
@@ -11003,7 +11017,7 @@
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -11015,14 +11029,14 @@
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
-      <c r="H5" s="74" t="n">
+      <c r="H5" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J5" s="62"/>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L5" s="51"/>
@@ -11033,7 +11047,7 @@
       <c r="O5" s="62"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="51"/>
-      <c r="R5" s="74"/>
+      <c r="R5" s="75"/>
       <c r="S5" s="62"/>
       <c r="T5" s="62"/>
     </row>
@@ -11041,7 +11055,7 @@
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -11055,14 +11069,14 @@
       <c r="G6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="74" t="n">
+      <c r="H6" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J6" s="62"/>
-      <c r="K6" s="74" t="s">
+      <c r="K6" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L6" s="51"/>
@@ -11073,7 +11087,7 @@
       <c r="O6" s="62"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
-      <c r="R6" s="74"/>
+      <c r="R6" s="75"/>
       <c r="S6" s="62"/>
       <c r="T6" s="62"/>
     </row>
@@ -11081,7 +11095,7 @@
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -11093,14 +11107,14 @@
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="74" t="n">
+      <c r="H7" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J7" s="62"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L7" s="51"/>
@@ -11111,7 +11125,7 @@
       <c r="O7" s="62"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
-      <c r="R7" s="74"/>
+      <c r="R7" s="75"/>
       <c r="S7" s="62"/>
       <c r="T7" s="62"/>
     </row>
@@ -11119,7 +11133,7 @@
       <c r="A8" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="74"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -11131,14 +11145,14 @@
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
-      <c r="H8" s="74" t="n">
+      <c r="H8" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J8" s="62"/>
-      <c r="K8" s="74" t="s">
+      <c r="K8" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L8" s="51"/>
@@ -11149,7 +11163,7 @@
       <c r="O8" s="62"/>
       <c r="P8" s="62"/>
       <c r="Q8" s="51"/>
-      <c r="R8" s="74"/>
+      <c r="R8" s="75"/>
       <c r="S8" s="62"/>
       <c r="T8" s="62"/>
     </row>
@@ -11157,7 +11171,7 @@
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -11169,14 +11183,14 @@
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="74" t="n">
+      <c r="H9" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="84" t="s">
+      <c r="I9" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J9" s="62"/>
-      <c r="K9" s="74" t="s">
+      <c r="K9" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L9" s="51"/>
@@ -11187,7 +11201,7 @@
       <c r="O9" s="62"/>
       <c r="P9" s="62"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="74"/>
+      <c r="R9" s="75"/>
       <c r="S9" s="62"/>
       <c r="T9" s="62"/>
     </row>
@@ -11195,7 +11209,7 @@
       <c r="A10" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="74"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -11207,14 +11221,14 @@
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="74" t="n">
+      <c r="H10" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J10" s="62"/>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L10" s="51"/>
@@ -11225,7 +11239,7 @@
       <c r="O10" s="62"/>
       <c r="P10" s="62"/>
       <c r="Q10" s="51"/>
-      <c r="R10" s="74"/>
+      <c r="R10" s="75"/>
       <c r="S10" s="62"/>
       <c r="T10" s="62"/>
     </row>
@@ -11233,26 +11247,26 @@
       <c r="A11" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="74"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
         <v>92</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="74" t="n">
+      <c r="H11" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J11" s="62"/>
-      <c r="K11" s="74" t="s">
+      <c r="K11" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L11" s="51"/>
@@ -11263,7 +11277,7 @@
       <c r="O11" s="62"/>
       <c r="P11" s="62"/>
       <c r="Q11" s="51"/>
-      <c r="R11" s="74"/>
+      <c r="R11" s="75"/>
       <c r="S11" s="62"/>
       <c r="T11" s="62"/>
     </row>
@@ -11271,7 +11285,7 @@
       <c r="A12" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="74"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -11283,14 +11297,14 @@
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="74" t="n">
+      <c r="H12" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J12" s="62"/>
-      <c r="K12" s="74" t="s">
+      <c r="K12" s="75" t="s">
         <v>198</v>
       </c>
       <c r="L12" s="51"/>
@@ -11301,7 +11315,7 @@
       <c r="O12" s="62"/>
       <c r="P12" s="62"/>
       <c r="Q12" s="51"/>
-      <c r="R12" s="74"/>
+      <c r="R12" s="75"/>
       <c r="S12" s="62"/>
       <c r="T12" s="62"/>
     </row>
@@ -11309,7 +11323,7 @@
       <c r="A13" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="74"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -11319,16 +11333,16 @@
       <c r="E13" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="74" t="n">
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="84" t="s">
+      <c r="I13" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J13" s="62"/>
-      <c r="K13" s="74" t="s">
+      <c r="K13" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L13" s="51"/>
@@ -11339,7 +11353,7 @@
       <c r="O13" s="62"/>
       <c r="P13" s="62"/>
       <c r="Q13" s="51"/>
-      <c r="R13" s="74"/>
+      <c r="R13" s="75"/>
       <c r="S13" s="62"/>
       <c r="T13" s="62"/>
     </row>
@@ -11347,7 +11361,7 @@
       <c r="A14" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="74"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -11359,14 +11373,14 @@
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
-      <c r="H14" s="74" t="n">
+      <c r="H14" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="84" t="s">
+      <c r="I14" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J14" s="62"/>
-      <c r="K14" s="74" t="s">
+      <c r="K14" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L14" s="51"/>
@@ -11377,7 +11391,7 @@
       <c r="O14" s="62"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
-      <c r="R14" s="74"/>
+      <c r="R14" s="75"/>
       <c r="S14" s="62"/>
       <c r="T14" s="62"/>
     </row>
@@ -11385,7 +11399,7 @@
       <c r="A15" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -11397,14 +11411,14 @@
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
-      <c r="H15" s="74" t="n">
+      <c r="H15" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="84" t="s">
+      <c r="I15" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J15" s="62"/>
-      <c r="K15" s="74" t="s">
+      <c r="K15" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L15" s="51"/>
@@ -11415,7 +11429,7 @@
       <c r="O15" s="62"/>
       <c r="P15" s="62"/>
       <c r="Q15" s="51"/>
-      <c r="R15" s="74"/>
+      <c r="R15" s="75"/>
       <c r="S15" s="62"/>
       <c r="T15" s="62"/>
     </row>
@@ -11423,7 +11437,7 @@
       <c r="A16" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="74"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -11435,14 +11449,14 @@
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
-      <c r="H16" s="74" t="n">
+      <c r="H16" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="84" t="s">
+      <c r="I16" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J16" s="62"/>
-      <c r="K16" s="74" t="s">
+      <c r="K16" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L16" s="51"/>
@@ -11453,7 +11467,7 @@
       <c r="O16" s="62"/>
       <c r="P16" s="62"/>
       <c r="Q16" s="51"/>
-      <c r="R16" s="74"/>
+      <c r="R16" s="75"/>
       <c r="S16" s="62"/>
       <c r="T16" s="62"/>
     </row>
@@ -11461,7 +11475,7 @@
       <c r="A17" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="74"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -11473,14 +11487,14 @@
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
-      <c r="H17" s="74" t="n">
+      <c r="H17" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="84" t="s">
+      <c r="I17" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J17" s="62"/>
-      <c r="K17" s="74" t="s">
+      <c r="K17" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L17" s="51"/>
@@ -11491,7 +11505,7 @@
       <c r="O17" s="62"/>
       <c r="P17" s="62"/>
       <c r="Q17" s="51"/>
-      <c r="R17" s="74"/>
+      <c r="R17" s="75"/>
       <c r="S17" s="62"/>
       <c r="T17" s="62"/>
     </row>
@@ -11499,7 +11513,7 @@
       <c r="A18" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="74"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -11511,14 +11525,14 @@
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
-      <c r="H18" s="74" t="n">
+      <c r="H18" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="84" t="s">
+      <c r="I18" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J18" s="62"/>
-      <c r="K18" s="74" t="s">
+      <c r="K18" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L18" s="51"/>
@@ -11529,7 +11543,7 @@
       <c r="O18" s="62"/>
       <c r="P18" s="62"/>
       <c r="Q18" s="51"/>
-      <c r="R18" s="74"/>
+      <c r="R18" s="75"/>
       <c r="S18" s="62"/>
       <c r="T18" s="62"/>
     </row>
@@ -11537,7 +11551,7 @@
       <c r="A19" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="74"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -11549,14 +11563,14 @@
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
-      <c r="H19" s="74" t="n">
+      <c r="H19" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="84" t="s">
+      <c r="I19" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J19" s="62"/>
-      <c r="K19" s="74" t="s">
+      <c r="K19" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L19" s="51"/>
@@ -11567,7 +11581,7 @@
       <c r="O19" s="62"/>
       <c r="P19" s="62"/>
       <c r="Q19" s="51"/>
-      <c r="R19" s="74"/>
+      <c r="R19" s="75"/>
       <c r="S19" s="62"/>
       <c r="T19" s="62"/>
     </row>
@@ -11575,26 +11589,26 @@
       <c r="A20" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="74"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="87" t="s">
         <v>90</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
-      <c r="H20" s="74" t="n">
+      <c r="H20" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="84" t="s">
+      <c r="I20" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J20" s="62"/>
-      <c r="K20" s="74" t="s">
+      <c r="K20" s="75" t="s">
         <v>199</v>
       </c>
       <c r="L20" s="51"/>
@@ -11605,7 +11619,7 @@
       <c r="O20" s="62"/>
       <c r="P20" s="62"/>
       <c r="Q20" s="51"/>
-      <c r="R20" s="74"/>
+      <c r="R20" s="75"/>
       <c r="S20" s="62"/>
       <c r="T20" s="62"/>
     </row>
@@ -11613,7 +11627,7 @@
       <c r="A21" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -11625,14 +11639,14 @@
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
-      <c r="H21" s="74" t="n">
+      <c r="H21" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="84" t="s">
+      <c r="I21" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J21" s="62"/>
-      <c r="K21" s="74" t="s">
+      <c r="K21" s="75" t="s">
         <v>200</v>
       </c>
       <c r="L21" s="51"/>
@@ -11643,7 +11657,7 @@
       <c r="O21" s="62"/>
       <c r="P21" s="62"/>
       <c r="Q21" s="51"/>
-      <c r="R21" s="74"/>
+      <c r="R21" s="75"/>
       <c r="S21" s="62"/>
       <c r="T21" s="62"/>
     </row>
@@ -11651,7 +11665,7 @@
       <c r="A22" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="74"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -11663,14 +11677,14 @@
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
-      <c r="H22" s="74" t="n">
+      <c r="H22" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="84" t="s">
+      <c r="I22" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J22" s="62"/>
-      <c r="K22" s="74" t="s">
+      <c r="K22" s="75" t="s">
         <v>200</v>
       </c>
       <c r="L22" s="51"/>
@@ -11681,7 +11695,7 @@
       <c r="O22" s="62"/>
       <c r="P22" s="62"/>
       <c r="Q22" s="51"/>
-      <c r="R22" s="74"/>
+      <c r="R22" s="75"/>
       <c r="S22" s="62"/>
       <c r="T22" s="62"/>
     </row>
@@ -11689,7 +11703,7 @@
       <c r="A23" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="74"/>
+      <c r="B23" s="75"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -11701,10 +11715,10 @@
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="74" t="n">
+      <c r="H23" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="86" t="s">
+      <c r="I23" s="88" t="s">
         <v>201</v>
       </c>
       <c r="J23" s="62"/>
@@ -11719,137 +11733,137 @@
       <c r="O23" s="62"/>
       <c r="P23" s="62"/>
       <c r="Q23" s="51"/>
-      <c r="R23" s="74"/>
+      <c r="R23" s="75"/>
       <c r="S23" s="62"/>
       <c r="T23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="87"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="Q24" s="88"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="Q24" s="90"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="Q25" s="88"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="Q25" s="90"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="Q26" s="88"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="Q26" s="90"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="87"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="Q27" s="88"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="Q27" s="90"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="87"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="88"/>
-      <c r="Q28" s="88"/>
+      <c r="A28" s="89"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="90"/>
+      <c r="Q28" s="90"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="87"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="Q29" s="88"/>
+      <c r="A29" s="89"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="Q29" s="90"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="87"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="Q30" s="88"/>
+      <c r="A30" s="89"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="Q30" s="90"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="87"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="Q31" s="88"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="90"/>
+      <c r="Q31" s="90"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="87"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="Q32" s="88"/>
+      <c r="A32" s="89"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="Q32" s="90"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="87"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="89"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="Q33" s="88"/>
+      <c r="A33" s="89"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="Q33" s="90"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="87"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="Q34" s="88"/>
+      <c r="A34" s="89"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="91"/>
+      <c r="G34" s="91"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="Q34" s="90"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix case definition error
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -1211,11 +1211,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1227,6 +1222,11 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1478,7 +1478,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1739,10 +1739,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1803,7 +1799,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1811,7 +1807,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1823,11 +1819,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2011,7 +2007,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2031,7 +2027,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2426,37 +2422,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="91" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2608,10 +2604,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2636,10 +2632,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2664,10 +2660,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="94" t="s">
+      <c r="E6" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2692,10 +2688,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="95" t="s">
+      <c r="F7" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2720,10 +2716,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="94" t="s">
+      <c r="E8" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2748,16 +2744,16 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="87" t="s">
+      <c r="H9" s="52" t="s">
         <v>90</v>
       </c>
       <c r="I9" s="62" t="n">
@@ -2776,10 +2772,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="93" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="94" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2796,9 +2792,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="90"/>
+      <c r="H11" s="89"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2827,184 +2823,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="96" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="96" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="96" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="96" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="96" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="96" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="96" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="96" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="96" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="95" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="95" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="104" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="105"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="109" t="s">
+      <c r="F3" s="108" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="109" t="s">
+      <c r="G3" s="108" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="110" t="s">
+      <c r="H3" s="109" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="110" t="s">
+      <c r="I3" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="110" t="s">
+      <c r="J3" s="109" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="110" t="s">
+      <c r="K3" s="109" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="110"/>
-      <c r="M3" s="111"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="110"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="112"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="112"/>
-      <c r="B6" s="112"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="112"/>
-      <c r="B7" s="112"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="111"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="112"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3047,20 +3043,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="114" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3102,10 +3098,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="116" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3131,11 +3127,11 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="52" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="51"/>
@@ -3143,7 +3139,7 @@
         <v>91</v>
       </c>
       <c r="G4" s="50"/>
-      <c r="H4" s="75" t="n">
+      <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="50"/>
@@ -3165,7 +3161,7 @@
         <v>76</v>
       </c>
       <c r="G5" s="50"/>
-      <c r="H5" s="75" t="n">
+      <c r="H5" s="74" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="50"/>
@@ -3187,7 +3183,7 @@
         <v>87</v>
       </c>
       <c r="G6" s="50"/>
-      <c r="H6" s="75" t="n">
+      <c r="H6" s="74" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="50"/>
@@ -3209,7 +3205,7 @@
         <v>89</v>
       </c>
       <c r="G7" s="50"/>
-      <c r="H7" s="75" t="n">
+      <c r="H7" s="74" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="50"/>
@@ -3231,7 +3227,7 @@
         <v>85</v>
       </c>
       <c r="G8" s="50"/>
-      <c r="H8" s="75" t="n">
+      <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
       <c r="I8" s="50"/>
@@ -3253,44 +3249,44 @@
         <v>80</v>
       </c>
       <c r="G9" s="62"/>
-      <c r="H9" s="75" t="n">
+      <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
       <c r="I9" s="62"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="66"/>
+      <c r="E10" s="65"/>
     </row>
     <row r="11" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="66"/>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="66"/>
+      <c r="E12" s="65"/>
     </row>
     <row r="13" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="66"/>
+      <c r="E13" s="65"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="66"/>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="66"/>
+      <c r="E15" s="65"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="66"/>
+      <c r="E16" s="65"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="66"/>
+      <c r="E17" s="65"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="66"/>
+      <c r="E18" s="65"/>
     </row>
     <row r="19" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="66"/>
+      <c r="E19" s="65"/>
     </row>
     <row r="20" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="66"/>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3348,7 +3344,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="69"/>
+      <c r="I1" s="68"/>
     </row>
     <row r="2" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -3375,48 +3371,48 @@
       <c r="H2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="119" t="s">
+      <c r="I2" s="118" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="120"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="123" t="s">
+      <c r="I3" s="122" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="124"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
-    </row>
-    <row r="4" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J3" s="123"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
+    </row>
+    <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3424,25 +3420,25 @@
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="52" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="75" t="n">
+      <c r="G4" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-    </row>
-    <row r="5" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+    </row>
+    <row r="5" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -3453,18 +3449,18 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="75" t="n">
+      <c r="G5" s="74" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-    </row>
-    <row r="6" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -3475,18 +3471,18 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="75" t="n">
+      <c r="G6" s="74" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-    </row>
-    <row r="7" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+    </row>
+    <row r="7" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -3497,14 +3493,14 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="75" t="n">
+      <c r="G7" s="74" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-    </row>
-    <row r="8" s="68" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+    </row>
+    <row r="8" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3519,14 +3515,14 @@
       <c r="F8" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="75" t="n">
+      <c r="G8" s="74" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="126" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="125" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3541,7 +3537,7 @@
       <c r="F9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="75" t="n">
+      <c r="G9" s="74" t="n">
         <v>7</v>
       </c>
       <c r="H9" s="25"/>
@@ -3549,26 +3545,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="127"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="127"/>
+      <c r="G11" s="126"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="89"/>
-      <c r="G12" s="127"/>
+      <c r="A12" s="88"/>
+      <c r="G12" s="126"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89"/>
-      <c r="G13" s="127"/>
+      <c r="A13" s="88"/>
+      <c r="G13" s="126"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89"/>
-      <c r="G14" s="127"/>
+      <c r="A14" s="88"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3608,7 +3604,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="127" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3617,60 +3613,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="129" t="s">
+      <c r="D1" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="130" t="s">
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="129" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="129" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="90" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="C3" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="131" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="131" t="s">
+      <c r="E3" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="131" t="s">
+      <c r="F3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="131" t="s">
+      <c r="G3" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="131" t="s">
+      <c r="H3" s="130" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="131" t="s">
+      <c r="I3" s="130" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3699,35 +3695,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="133" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="133" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="132" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="132" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="133" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="133" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="133" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="132" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="132" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="133" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="135" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3763,34 +3759,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="91" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3806,11 +3802,11 @@
         <v>90</v>
       </c>
       <c r="E4" s="52"/>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75" t="n">
+      <c r="G4" s="74"/>
+      <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="50"/>
@@ -3820,7 +3816,7 @@
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -3831,8 +3827,8 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75" t="n">
+      <c r="G5" s="74"/>
+      <c r="H5" s="74" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="50"/>
@@ -3842,7 +3838,7 @@
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -3853,8 +3849,8 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75" t="n">
+      <c r="G6" s="74"/>
+      <c r="H6" s="74" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="50"/>
@@ -3864,7 +3860,7 @@
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -3875,8 +3871,8 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75" t="n">
+      <c r="G7" s="74"/>
+      <c r="H7" s="74" t="n">
         <v>4</v>
       </c>
       <c r="I7" s="50"/>
@@ -3898,10 +3894,10 @@
         <v>85</v>
       </c>
       <c r="G8" s="25"/>
-      <c r="H8" s="75" t="n">
+      <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="138"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3912,7 +3908,7 @@
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="52" t="s">
         <v>79</v>
       </c>
       <c r="E9" s="25"/>
@@ -3920,10 +3916,10 @@
         <v>80</v>
       </c>
       <c r="G9" s="25"/>
-      <c r="H9" s="75" t="n">
+      <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="138"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3942,10 +3938,10 @@
         <v>257</v>
       </c>
       <c r="G10" s="25"/>
-      <c r="H10" s="75" t="n">
+      <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="138"/>
+      <c r="I10" s="137"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4034,37 +4030,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="122" t="s">
+      <c r="D3" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="91" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4074,14 +4070,14 @@
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="52" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="75" t="n">
+      <c r="G4" s="74" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="50"/>
@@ -4103,7 +4099,7 @@
       <c r="F5" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="75" t="n">
+      <c r="G5" s="74" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="50"/>
@@ -4125,7 +4121,7 @@
       <c r="F6" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="75" t="n">
+      <c r="G6" s="74" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="50"/>
@@ -4147,7 +4143,7 @@
       <c r="F7" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="75" t="n">
+      <c r="G7" s="74" t="n">
         <v>4</v>
       </c>
       <c r="H7" s="50"/>
@@ -4169,7 +4165,7 @@
       <c r="F8" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="75" t="n">
+      <c r="G8" s="74" t="n">
         <v>6</v>
       </c>
       <c r="H8" s="50"/>
@@ -4191,7 +4187,7 @@
       <c r="F9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="75" t="n">
+      <c r="G9" s="74" t="n">
         <v>7</v>
       </c>
       <c r="H9" s="50"/>
@@ -4213,7 +4209,7 @@
       <c r="F10" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="G10" s="75" t="n">
+      <c r="G10" s="74" t="n">
         <v>8</v>
       </c>
       <c r="H10" s="50"/>
@@ -4221,32 +4217,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="139"/>
-      <c r="D11" s="139"/>
-      <c r="F11" s="139"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
+      <c r="F11" s="138"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="89"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="F12" s="139"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="F12" s="138"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="F13" s="139"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="F13" s="138"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="139"/>
-      <c r="D14" s="139"/>
-      <c r="F14" s="139"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="F14" s="138"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4328,13 +4324,13 @@
       <c r="C3" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="79" t="s">
         <v>265</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="79" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4343,10 +4339,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="139" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="139" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4357,8 +4353,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89"/>
-      <c r="C5" s="141"/>
+      <c r="A5" s="88"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4431,31 +4427,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="142" t="s">
+      <c r="D3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4668,7 +4664,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4711,8 +4707,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4728,7 +4724,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="142" t="s">
         <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4740,12 +4736,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4766,42 +4762,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="145" t="s">
+      <c r="A3" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="145" t="s">
+      <c r="B3" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="145" t="s">
+      <c r="F3" s="144" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4828,7 +4824,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4846,7 +4842,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4864,7 +4860,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4882,7 +4878,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="118"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4900,7 +4896,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="118"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4918,7 +4914,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="118"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4936,11 +4932,11 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="118"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="52" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -4954,7 +4950,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="118"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4972,7 +4968,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="118"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -5094,13 +5090,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5111,7 +5107,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5129,7 +5125,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5147,7 +5143,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="118"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5165,7 +5161,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="118"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5211,31 +5207,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="148" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="148" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="152" t="s">
+      <c r="D1" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5247,7 +5243,7 @@
       <c r="C2" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="153" t="s">
         <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5256,29 +5252,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="147" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="147" t="s">
+      <c r="D3" s="146" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="155" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5332,7 +5328,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5384,10 +5380,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="48" t="s">
@@ -5399,10 +5395,10 @@
       <c r="E3" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="76" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5494,73 +5490,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="126" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="126" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="126" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="126" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="126" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="125" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="125" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="156" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="159"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="159" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="159" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="159" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="160" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="160" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="160" t="s">
         <v>295</v>
       </c>
-      <c r="D3" s="161" t="s">
+      <c r="D3" s="160" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="4" s="68" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="162" t="s">
+    <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="161" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="162" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="162" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="5" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="164"/>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="166"/>
-    </row>
-    <row r="6" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="68" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="165"/>
+    </row>
+    <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7160,7 +7156,7 @@
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="64" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -7643,13 +7639,13 @@
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="55"/>
       <c r="C14" s="56"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="53"/>
-      <c r="J14" s="67"/>
+      <c r="J14" s="66"/>
       <c r="K14" s="53"/>
       <c r="L14" s="53"/>
       <c r="M14" s="53"/>
@@ -8035,10 +8031,10 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="67"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="66"/>
       <c r="AHE16" s="0"/>
       <c r="AHF16" s="0"/>
       <c r="AHG16" s="0"/>
@@ -8177,9 +8173,9 @@
       <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="68"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="67"/>
       <c r="AHE17" s="0"/>
       <c r="AHF17" s="0"/>
       <c r="AHG17" s="0"/>
@@ -8318,10 +8314,10 @@
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="67"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="66"/>
       <c r="AHE18" s="0"/>
       <c r="AHF18" s="0"/>
       <c r="AHG18" s="0"/>
@@ -8460,8 +8456,8 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="66"/>
-      <c r="E19" s="67"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="66"/>
       <c r="AHE19" s="0"/>
       <c r="AHF19" s="0"/>
       <c r="AHG19" s="0"/>
@@ -8600,8 +8596,8 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
       <c r="AHE20" s="0"/>
       <c r="AHF20" s="0"/>
       <c r="AHG20" s="0"/>
@@ -8740,8 +8736,8 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
       <c r="AHE21" s="0"/>
       <c r="AHF21" s="0"/>
       <c r="AHG21" s="0"/>
@@ -8880,8 +8876,8 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
       <c r="AHE22" s="0"/>
       <c r="AHF22" s="0"/>
       <c r="AHG22" s="0"/>
@@ -9020,8 +9016,8 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
       <c r="AHE23" s="0"/>
       <c r="AHF23" s="0"/>
       <c r="AHG23" s="0"/>
@@ -9160,11 +9156,11 @@
       <c r="AMJ23" s="0"/>
     </row>
     <row r="24" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
       <c r="F24" s="53"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="65"/>
       <c r="AHE24" s="0"/>
       <c r="AHF24" s="0"/>
       <c r="AHG24" s="0"/>
@@ -9303,8 +9299,8 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
       <c r="AHE25" s="0"/>
       <c r="AHF25" s="0"/>
       <c r="AHG25" s="0"/>
@@ -9508,7 +9504,7 @@
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
-      <c r="O1" s="69"/>
+      <c r="O1" s="68"/>
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -9553,10 +9549,10 @@
       <c r="N2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="70" t="s">
+      <c r="O2" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="71"/>
+      <c r="P2" s="70"/>
       <c r="Q2" s="47"/>
       <c r="R2" s="47"/>
     </row>
@@ -9567,10 +9563,10 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="71" t="s">
         <v>106</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -9603,10 +9599,10 @@
       <c r="N3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="73" t="s">
+      <c r="O3" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="74"/>
+      <c r="P3" s="73"/>
       <c r="Q3" s="61"/>
       <c r="R3" s="61"/>
     </row>
@@ -9629,7 +9625,7 @@
         <v>112</v>
       </c>
       <c r="H4" s="62"/>
-      <c r="I4" s="75"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="62"/>
       <c r="K4" s="51" t="s">
         <v>41</v>
@@ -10182,75 +10178,75 @@
       <c r="IU6" s="53"/>
     </row>
     <row r="7" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="53"/>
-      <c r="G7" s="66"/>
+      <c r="G7" s="65"/>
     </row>
     <row r="8" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="53"/>
-      <c r="G8" s="66"/>
-      <c r="I8" s="76"/>
+      <c r="G8" s="65"/>
+      <c r="I8" s="75"/>
     </row>
     <row r="9" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
       <c r="F9" s="53"/>
-      <c r="G9" s="66"/>
+      <c r="G9" s="65"/>
     </row>
     <row r="10" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
       <c r="F10" s="53"/>
-      <c r="G10" s="66"/>
-      <c r="J10" s="67"/>
+      <c r="G10" s="65"/>
+      <c r="J10" s="66"/>
     </row>
     <row r="11" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="53"/>
-      <c r="G11" s="66"/>
-      <c r="I11" s="76"/>
+      <c r="G11" s="65"/>
+      <c r="I11" s="75"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="53"/>
-      <c r="G12" s="66"/>
-      <c r="J12" s="67"/>
+      <c r="G12" s="65"/>
+      <c r="J12" s="66"/>
     </row>
     <row r="13" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="66"/>
+      <c r="G13" s="65"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="66"/>
-      <c r="J14" s="67"/>
+      <c r="G14" s="65"/>
+      <c r="J14" s="66"/>
     </row>
     <row r="15" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
       <c r="F15" s="53"/>
-      <c r="G15" s="66"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
       <c r="F16" s="53"/>
-      <c r="G16" s="66"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
       <c r="F17" s="53"/>
-      <c r="G17" s="66"/>
+      <c r="G17" s="65"/>
     </row>
     <row r="18" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -10341,7 +10337,7 @@
       <c r="E3" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="76" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="61"/>
@@ -10357,10 +10353,10 @@
       <c r="C4" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="77" t="s">
         <v>126</v>
       </c>
       <c r="F4" s="62" t="n">
@@ -10375,10 +10371,10 @@
       <c r="C5" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="77" t="s">
         <v>127</v>
       </c>
       <c r="F5" s="62" t="n">
@@ -10452,12 +10448,12 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
       <c r="R1" s="15"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
@@ -10547,10 +10543,10 @@
       <c r="G3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="I3" s="79" t="s">
         <v>142</v>
       </c>
       <c r="J3" s="20" t="s">
@@ -10577,13 +10573,13 @@
       <c r="R3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="S3" s="77" t="s">
+      <c r="S3" s="76" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="77" t="s">
+      <c r="T3" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="U3" s="77" t="s">
+      <c r="U3" s="76" t="s">
         <v>152</v>
       </c>
     </row>
@@ -10620,8 +10616,8 @@
       <c r="N4" s="50"/>
       <c r="O4" s="50"/>
       <c r="P4" s="50"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81" t="s">
+      <c r="R4" s="80"/>
+      <c r="S4" s="80" t="s">
         <v>156</v>
       </c>
       <c r="T4" s="50"/>
@@ -10662,8 +10658,8 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81" t="s">
+      <c r="R5" s="80"/>
+      <c r="S5" s="80" t="s">
         <v>156</v>
       </c>
       <c r="T5" s="50"/>
@@ -10704,8 +10700,8 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81" t="s">
+      <c r="R6" s="80"/>
+      <c r="S6" s="80" t="s">
         <v>156</v>
       </c>
       <c r="T6" s="50"/>
@@ -10740,20 +10736,20 @@
       <c r="J7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="81"/>
       <c r="L7" s="50" t="n">
         <v>5</v>
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="83" t="s">
+      <c r="O7" s="82" t="s">
         <v>166</v>
       </c>
       <c r="P7" s="50"/>
-      <c r="R7" s="81" t="s">
+      <c r="R7" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="S7" s="81" t="s">
+      <c r="S7" s="80" t="s">
         <v>156</v>
       </c>
       <c r="T7" s="50"/>
@@ -10780,8 +10776,8 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10959,7 +10955,7 @@
       <c r="O3" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="84" t="s">
+      <c r="P3" s="83" t="s">
         <v>192</v>
       </c>
       <c r="Q3" s="21" t="s">
@@ -10979,7 +10975,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -10991,14 +10987,14 @@
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
-      <c r="H4" s="75" t="n">
+      <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="85" t="s">
+      <c r="I4" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J4" s="62"/>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L4" s="51"/>
@@ -11009,7 +11005,7 @@
       <c r="O4" s="62"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="51"/>
-      <c r="R4" s="75"/>
+      <c r="R4" s="74"/>
       <c r="S4" s="62"/>
       <c r="T4" s="62"/>
     </row>
@@ -11017,7 +11013,7 @@
       <c r="A5" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -11029,14 +11025,14 @@
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
-      <c r="H5" s="75" t="n">
+      <c r="H5" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="85" t="s">
+      <c r="I5" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J5" s="62"/>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L5" s="51"/>
@@ -11047,7 +11043,7 @@
       <c r="O5" s="62"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="51"/>
-      <c r="R5" s="75"/>
+      <c r="R5" s="74"/>
       <c r="S5" s="62"/>
       <c r="T5" s="62"/>
     </row>
@@ -11055,7 +11051,7 @@
       <c r="A6" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -11069,14 +11065,14 @@
       <c r="G6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="75" t="n">
+      <c r="H6" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="85" t="s">
+      <c r="I6" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J6" s="62"/>
-      <c r="K6" s="75" t="s">
+      <c r="K6" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L6" s="51"/>
@@ -11087,7 +11083,7 @@
       <c r="O6" s="62"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
-      <c r="R6" s="75"/>
+      <c r="R6" s="74"/>
       <c r="S6" s="62"/>
       <c r="T6" s="62"/>
     </row>
@@ -11095,7 +11091,7 @@
       <c r="A7" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="75"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -11107,14 +11103,14 @@
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
-      <c r="H7" s="75" t="n">
+      <c r="H7" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="85" t="s">
+      <c r="I7" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J7" s="62"/>
-      <c r="K7" s="75" t="s">
+      <c r="K7" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L7" s="51"/>
@@ -11125,7 +11121,7 @@
       <c r="O7" s="62"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
-      <c r="R7" s="75"/>
+      <c r="R7" s="74"/>
       <c r="S7" s="62"/>
       <c r="T7" s="62"/>
     </row>
@@ -11133,7 +11129,7 @@
       <c r="A8" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="75"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -11145,14 +11141,14 @@
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
-      <c r="H8" s="75" t="n">
+      <c r="H8" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="85" t="s">
+      <c r="I8" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J8" s="62"/>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L8" s="51"/>
@@ -11163,7 +11159,7 @@
       <c r="O8" s="62"/>
       <c r="P8" s="62"/>
       <c r="Q8" s="51"/>
-      <c r="R8" s="75"/>
+      <c r="R8" s="74"/>
       <c r="S8" s="62"/>
       <c r="T8" s="62"/>
     </row>
@@ -11171,7 +11167,7 @@
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -11183,14 +11179,14 @@
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
-      <c r="H9" s="75" t="n">
+      <c r="H9" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J9" s="62"/>
-      <c r="K9" s="75" t="s">
+      <c r="K9" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L9" s="51"/>
@@ -11201,7 +11197,7 @@
       <c r="O9" s="62"/>
       <c r="P9" s="62"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="75"/>
+      <c r="R9" s="74"/>
       <c r="S9" s="62"/>
       <c r="T9" s="62"/>
     </row>
@@ -11209,7 +11205,7 @@
       <c r="A10" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="75"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -11221,14 +11217,14 @@
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="75" t="n">
+      <c r="H10" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="85" t="s">
+      <c r="I10" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J10" s="62"/>
-      <c r="K10" s="75" t="s">
+      <c r="K10" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L10" s="51"/>
@@ -11239,7 +11235,7 @@
       <c r="O10" s="62"/>
       <c r="P10" s="62"/>
       <c r="Q10" s="51"/>
-      <c r="R10" s="75"/>
+      <c r="R10" s="74"/>
       <c r="S10" s="62"/>
       <c r="T10" s="62"/>
     </row>
@@ -11247,26 +11243,26 @@
       <c r="A11" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="75"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="52" t="s">
-        <v>90</v>
+      <c r="D11" s="85" t="s">
+        <v>153</v>
       </c>
       <c r="E11" s="52" t="s">
         <v>92</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="75" t="n">
+      <c r="H11" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J11" s="62"/>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L11" s="51"/>
@@ -11277,7 +11273,7 @@
       <c r="O11" s="62"/>
       <c r="P11" s="62"/>
       <c r="Q11" s="51"/>
-      <c r="R11" s="75"/>
+      <c r="R11" s="74"/>
       <c r="S11" s="62"/>
       <c r="T11" s="62"/>
     </row>
@@ -11285,7 +11281,7 @@
       <c r="A12" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="75"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -11297,14 +11293,14 @@
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
-      <c r="H12" s="75" t="n">
+      <c r="H12" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="85" t="s">
+      <c r="I12" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J12" s="62"/>
-      <c r="K12" s="75" t="s">
+      <c r="K12" s="74" t="s">
         <v>198</v>
       </c>
       <c r="L12" s="51"/>
@@ -11315,7 +11311,7 @@
       <c r="O12" s="62"/>
       <c r="P12" s="62"/>
       <c r="Q12" s="51"/>
-      <c r="R12" s="75"/>
+      <c r="R12" s="74"/>
       <c r="S12" s="62"/>
       <c r="T12" s="62"/>
     </row>
@@ -11323,7 +11319,7 @@
       <c r="A13" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="75"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -11335,14 +11331,14 @@
       </c>
       <c r="F13" s="86"/>
       <c r="G13" s="86"/>
-      <c r="H13" s="75" t="n">
+      <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J13" s="62"/>
-      <c r="K13" s="75" t="s">
+      <c r="K13" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L13" s="51"/>
@@ -11353,7 +11349,7 @@
       <c r="O13" s="62"/>
       <c r="P13" s="62"/>
       <c r="Q13" s="51"/>
-      <c r="R13" s="75"/>
+      <c r="R13" s="74"/>
       <c r="S13" s="62"/>
       <c r="T13" s="62"/>
     </row>
@@ -11361,7 +11357,7 @@
       <c r="A14" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
@@ -11373,14 +11369,14 @@
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
-      <c r="H14" s="75" t="n">
+      <c r="H14" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="85" t="s">
+      <c r="I14" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J14" s="62"/>
-      <c r="K14" s="75" t="s">
+      <c r="K14" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L14" s="51"/>
@@ -11391,7 +11387,7 @@
       <c r="O14" s="62"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
-      <c r="R14" s="75"/>
+      <c r="R14" s="74"/>
       <c r="S14" s="62"/>
       <c r="T14" s="62"/>
     </row>
@@ -11399,7 +11395,7 @@
       <c r="A15" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B15" s="75"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
@@ -11411,14 +11407,14 @@
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
-      <c r="H15" s="75" t="n">
+      <c r="H15" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J15" s="62"/>
-      <c r="K15" s="75" t="s">
+      <c r="K15" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L15" s="51"/>
@@ -11429,7 +11425,7 @@
       <c r="O15" s="62"/>
       <c r="P15" s="62"/>
       <c r="Q15" s="51"/>
-      <c r="R15" s="75"/>
+      <c r="R15" s="74"/>
       <c r="S15" s="62"/>
       <c r="T15" s="62"/>
     </row>
@@ -11437,7 +11433,7 @@
       <c r="A16" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B16" s="75"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="42" t="s">
         <v>38</v>
       </c>
@@ -11449,14 +11445,14 @@
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
-      <c r="H16" s="75" t="n">
+      <c r="H16" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="85" t="s">
+      <c r="I16" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J16" s="62"/>
-      <c r="K16" s="75" t="s">
+      <c r="K16" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L16" s="51"/>
@@ -11467,7 +11463,7 @@
       <c r="O16" s="62"/>
       <c r="P16" s="62"/>
       <c r="Q16" s="51"/>
-      <c r="R16" s="75"/>
+      <c r="R16" s="74"/>
       <c r="S16" s="62"/>
       <c r="T16" s="62"/>
     </row>
@@ -11475,7 +11471,7 @@
       <c r="A17" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B17" s="75"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="42" t="s">
         <v>38</v>
       </c>
@@ -11487,14 +11483,14 @@
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
-      <c r="H17" s="75" t="n">
+      <c r="H17" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="85" t="s">
+      <c r="I17" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J17" s="62"/>
-      <c r="K17" s="75" t="s">
+      <c r="K17" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L17" s="51"/>
@@ -11505,7 +11501,7 @@
       <c r="O17" s="62"/>
       <c r="P17" s="62"/>
       <c r="Q17" s="51"/>
-      <c r="R17" s="75"/>
+      <c r="R17" s="74"/>
       <c r="S17" s="62"/>
       <c r="T17" s="62"/>
     </row>
@@ -11513,7 +11509,7 @@
       <c r="A18" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="42" t="s">
         <v>38</v>
       </c>
@@ -11525,14 +11521,14 @@
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
-      <c r="H18" s="75" t="n">
+      <c r="H18" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="85" t="s">
+      <c r="I18" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J18" s="62"/>
-      <c r="K18" s="75" t="s">
+      <c r="K18" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L18" s="51"/>
@@ -11543,7 +11539,7 @@
       <c r="O18" s="62"/>
       <c r="P18" s="62"/>
       <c r="Q18" s="51"/>
-      <c r="R18" s="75"/>
+      <c r="R18" s="74"/>
       <c r="S18" s="62"/>
       <c r="T18" s="62"/>
     </row>
@@ -11551,7 +11547,7 @@
       <c r="A19" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B19" s="75"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="42" t="s">
         <v>38</v>
       </c>
@@ -11563,14 +11559,14 @@
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
-      <c r="H19" s="75" t="n">
+      <c r="H19" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J19" s="62"/>
-      <c r="K19" s="75" t="s">
+      <c r="K19" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L19" s="51"/>
@@ -11581,7 +11577,7 @@
       <c r="O19" s="62"/>
       <c r="P19" s="62"/>
       <c r="Q19" s="51"/>
-      <c r="R19" s="75"/>
+      <c r="R19" s="74"/>
       <c r="S19" s="62"/>
       <c r="T19" s="62"/>
     </row>
@@ -11589,26 +11585,26 @@
       <c r="A20" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="E20" s="87" t="s">
+      <c r="E20" s="52" t="s">
         <v>90</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
-      <c r="H20" s="75" t="n">
+      <c r="H20" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J20" s="62"/>
-      <c r="K20" s="75" t="s">
+      <c r="K20" s="74" t="s">
         <v>199</v>
       </c>
       <c r="L20" s="51"/>
@@ -11619,7 +11615,7 @@
       <c r="O20" s="62"/>
       <c r="P20" s="62"/>
       <c r="Q20" s="51"/>
-      <c r="R20" s="75"/>
+      <c r="R20" s="74"/>
       <c r="S20" s="62"/>
       <c r="T20" s="62"/>
     </row>
@@ -11627,7 +11623,7 @@
       <c r="A21" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B21" s="75"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="42" t="s">
         <v>38</v>
       </c>
@@ -11639,14 +11635,14 @@
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
-      <c r="H21" s="75" t="n">
+      <c r="H21" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="85" t="s">
+      <c r="I21" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J21" s="62"/>
-      <c r="K21" s="75" t="s">
+      <c r="K21" s="74" t="s">
         <v>200</v>
       </c>
       <c r="L21" s="51"/>
@@ -11657,7 +11653,7 @@
       <c r="O21" s="62"/>
       <c r="P21" s="62"/>
       <c r="Q21" s="51"/>
-      <c r="R21" s="75"/>
+      <c r="R21" s="74"/>
       <c r="S21" s="62"/>
       <c r="T21" s="62"/>
     </row>
@@ -11665,7 +11661,7 @@
       <c r="A22" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B22" s="75"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="42" t="s">
         <v>38</v>
       </c>
@@ -11677,14 +11673,14 @@
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
-      <c r="H22" s="75" t="n">
+      <c r="H22" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="85" t="s">
+      <c r="I22" s="84" t="s">
         <v>197</v>
       </c>
       <c r="J22" s="62"/>
-      <c r="K22" s="75" t="s">
+      <c r="K22" s="74" t="s">
         <v>200</v>
       </c>
       <c r="L22" s="51"/>
@@ -11695,7 +11691,7 @@
       <c r="O22" s="62"/>
       <c r="P22" s="62"/>
       <c r="Q22" s="51"/>
-      <c r="R22" s="75"/>
+      <c r="R22" s="74"/>
       <c r="S22" s="62"/>
       <c r="T22" s="62"/>
     </row>
@@ -11703,7 +11699,7 @@
       <c r="A23" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B23" s="75"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
@@ -11715,10 +11711,10 @@
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="75" t="n">
+      <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="88" t="s">
+      <c r="I23" s="87" t="s">
         <v>201</v>
       </c>
       <c r="J23" s="62"/>
@@ -11733,137 +11729,137 @@
       <c r="O23" s="62"/>
       <c r="P23" s="62"/>
       <c r="Q23" s="51"/>
-      <c r="R23" s="75"/>
+      <c r="R23" s="74"/>
       <c r="S23" s="62"/>
       <c r="T23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="89"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="Q24" s="90"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="Q24" s="89"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="89"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="Q25" s="90"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="Q25" s="89"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="Q26" s="90"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="Q26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="Q27" s="90"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="Q27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="90"/>
-      <c r="Q28" s="90"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="Q29" s="90"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="Q29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="89"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="Q30" s="90"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="Q30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="89"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="90"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="Q31" s="90"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="Q31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="Q32" s="90"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="Q32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="Q33" s="90"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="Q33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="89"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="90"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="Q34" s="90"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="Q34" s="89"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
revert to recordingReference field name
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">Court Location Code</t>
   </si>
   <si>
-    <t xml:space="preserve">caseReference</t>
+    <t xml:space="preserve">recordingReference</t>
   </si>
   <si>
     <t xml:space="preserve">Case Reference</t>
@@ -1043,7 +1043,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1222,11 +1222,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1465,7 +1460,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1478,7 +1473,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="165">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1819,10 +1814,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1927,6 +1918,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1935,7 +1930,27 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1943,15 +1958,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1963,15 +1970,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1979,7 +1982,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1987,46 +1998,26 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2039,7 +2030,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2047,7 +2038,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2127,7 +2118,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2135,11 +2126,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2422,37 +2413,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="90" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="90" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="91" t="s">
+      <c r="J3" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="91" t="s">
+      <c r="K3" s="90" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2604,10 +2595,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2632,10 +2623,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="93" t="s">
+      <c r="E5" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="94" t="s">
+      <c r="F5" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2660,10 +2651,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="93" t="s">
+      <c r="E6" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="94" t="s">
+      <c r="F6" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2688,10 +2679,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="93" t="s">
+      <c r="E7" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2716,10 +2707,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2744,10 +2735,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="93" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
@@ -2772,10 +2763,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="93" t="s">
+      <c r="E10" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="93" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2792,9 +2783,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
+      <c r="A11" s="87"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="89"/>
+      <c r="H11" s="88"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2823,184 +2814,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="95" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="95" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="94" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="94" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="94" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="94" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="94" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="94" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="94" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="94" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="94" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="103" t="s">
+      <c r="D2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="102" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="102" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="103" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="103" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="103" t="s">
+      <c r="J2" s="102" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="104"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="108" t="s">
+      <c r="E3" s="107" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="108" t="s">
+      <c r="F3" s="107" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="108" t="s">
+      <c r="G3" s="107" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="109" t="s">
+      <c r="H3" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="109" t="s">
+      <c r="I3" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="109" t="s">
+      <c r="K3" s="108" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="109"/>
-      <c r="M3" s="110"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="111"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="111"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
+      <c r="A5" s="110"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="111"/>
-      <c r="B6" s="111"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="110"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="111"/>
-      <c r="B7" s="111"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="110"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="99"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="111"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="99"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3043,20 +3034,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="113" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3098,10 +3089,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="115" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3127,7 +3118,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3371,46 +3362,46 @@
       <c r="H2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="118" t="s">
+      <c r="I2" s="117" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="121" t="s">
+      <c r="D3" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="122" t="s">
+      <c r="I3" s="121" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3522,7 +3513,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="125" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="124" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3545,26 +3536,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="88"/>
+      <c r="A10" s="87"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="126"/>
+      <c r="G10" s="125"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
+      <c r="A11" s="87"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="126"/>
+      <c r="G11" s="125"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88"/>
-      <c r="G12" s="126"/>
+      <c r="A12" s="87"/>
+      <c r="G12" s="125"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="88"/>
-      <c r="G13" s="126"/>
+      <c r="A13" s="87"/>
+      <c r="G13" s="125"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88"/>
-      <c r="G14" s="126"/>
+      <c r="A14" s="87"/>
+      <c r="G14" s="125"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3604,7 +3595,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="126" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3613,60 +3604,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="128" t="s">
+      <c r="D1" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="129" t="s">
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="129" t="s">
+      <c r="E2" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="131" t="s">
+      <c r="D3" s="130" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="130" t="s">
+      <c r="E3" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="130" t="s">
+      <c r="F3" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="130" t="s">
+      <c r="G3" s="129" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="130" t="s">
+      <c r="H3" s="129" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="130" t="s">
+      <c r="I3" s="129" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3695,35 +3686,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="132" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="132" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="131" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="131" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="131" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="132" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="132" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="132" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="131" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="131" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="131" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="132" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="135" t="s">
+      <c r="D1" s="134" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,34 +3750,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="91" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="91" t="s">
+      <c r="J3" s="90" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3897,7 +3888,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="137"/>
+      <c r="I8" s="136"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3919,7 +3910,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="137"/>
+      <c r="I9" s="136"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3941,7 +3932,7 @@
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="137"/>
+      <c r="I10" s="136"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4030,37 +4021,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="121" t="s">
+      <c r="D3" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="91" t="s">
+      <c r="H3" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="91" t="s">
+      <c r="I3" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="124"/>
-      <c r="K3" s="124"/>
-      <c r="L3" s="124"/>
-      <c r="M3" s="124"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4217,32 +4208,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="F11" s="138"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="137"/>
+      <c r="F11" s="137"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="F12" s="138"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="137"/>
+      <c r="F12" s="137"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="F13" s="138"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="F13" s="137"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="F14" s="138"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="F14" s="137"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4339,10 +4330,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="138" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="138" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4353,8 +4344,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88"/>
-      <c r="C5" s="140"/>
+      <c r="A5" s="87"/>
+      <c r="C5" s="139"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4427,31 +4418,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="140" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="88"/>
+      <c r="A4" s="87"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88"/>
+      <c r="A5" s="87"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4664,7 +4655,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4707,8 +4698,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4724,7 +4715,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="141" t="s">
         <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4736,12 +4727,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4762,42 +4753,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="144" t="s">
+      <c r="B3" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="144" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="144" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="144" t="s">
+      <c r="F3" s="143" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4824,7 +4815,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4842,7 +4833,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4860,7 +4851,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4878,7 +4869,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="117"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4896,7 +4887,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4914,7 +4905,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="117"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4932,7 +4923,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="117"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4950,7 +4941,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="117"/>
+      <c r="B12" s="116"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4968,7 +4959,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="117"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -5090,13 +5081,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="145" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5107,7 +5098,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="117"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5125,7 +5116,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="117"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5143,7 +5134,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="117"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5161,7 +5152,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5207,31 +5198,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="146" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="146" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="146" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="146" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="146" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="146" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="147" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="150" t="s">
+      <c r="C1" s="149" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5243,7 +5234,7 @@
       <c r="C2" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="153" t="s">
+      <c r="D2" s="152" t="s">
         <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5252,29 +5243,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="D3" s="145" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="155" t="s">
+      <c r="F3" s="154" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5490,57 +5481,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="125" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="125" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="124" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="124" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="158"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="157"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="158" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="158" t="s">
         <v>290</v>
       </c>
-      <c r="C2" s="159" t="s">
+      <c r="C2" s="158" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="159" t="s">
+      <c r="D2" s="158" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="159" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="159" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="160" t="s">
+      <c r="C3" s="159" t="s">
         <v>295</v>
       </c>
-      <c r="D3" s="160" t="s">
+      <c r="D3" s="159" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="160" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="161" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="C4" s="161" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -5548,10 +5539,10 @@
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="163"/>
-      <c r="B5" s="164"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="165"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="164"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10776,8 +10767,8 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11247,7 +11238,7 @@
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="52" t="s">
         <v>153</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -11329,8 +11320,8 @@
       <c r="E13" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
@@ -11714,7 +11705,7 @@
       <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="87" t="s">
+      <c r="I23" s="86" t="s">
         <v>201</v>
       </c>
       <c r="J23" s="62"/>
@@ -11734,132 +11725,132 @@
       <c r="T23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="88"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="89"/>
-      <c r="K24" s="89"/>
-      <c r="L24" s="89"/>
-      <c r="Q24" s="89"/>
+      <c r="A24" s="87"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="Q24" s="88"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="89"/>
-      <c r="G25" s="89"/>
-      <c r="K25" s="89"/>
-      <c r="L25" s="89"/>
-      <c r="Q25" s="89"/>
+      <c r="A25" s="87"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="Q25" s="88"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="88"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="89"/>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89"/>
-      <c r="Q26" s="89"/>
+      <c r="A26" s="87"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="Q26" s="88"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="88"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="Q27" s="89"/>
+      <c r="A27" s="87"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="Q27" s="88"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="88"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="O28" s="89"/>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="89"/>
+      <c r="A28" s="87"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="K28" s="88"/>
+      <c r="L28" s="88"/>
+      <c r="O28" s="88"/>
+      <c r="P28" s="88"/>
+      <c r="Q28" s="88"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="88"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="Q29" s="89"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="K29" s="88"/>
+      <c r="L29" s="88"/>
+      <c r="Q29" s="88"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="88"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-      <c r="Q30" s="89"/>
+      <c r="A30" s="87"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="Q30" s="88"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="88"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="89"/>
-      <c r="G31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
-      <c r="Q31" s="89"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="Q31" s="88"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="Q32" s="89"/>
+      <c r="A32" s="87"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="88"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="88"/>
+      <c r="Q32" s="88"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="88"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="89"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
-      <c r="K33" s="89"/>
-      <c r="L33" s="89"/>
-      <c r="Q33" s="89"/>
+      <c r="A33" s="87"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="88"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="Q33" s="88"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="88"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="90"/>
-      <c r="G34" s="90"/>
-      <c r="K34" s="89"/>
-      <c r="L34" s="89"/>
-      <c r="Q34" s="89"/>
+      <c r="A34" s="87"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="K34" s="88"/>
+      <c r="L34" s="88"/>
+      <c r="Q34" s="88"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
change segmentNumber into string in CCD
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -417,16 +417,16 @@
     <t xml:space="preserve">segmentNumber</t>
   </si>
   <si>
+    <t xml:space="preserve">Hearing File Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the file is split into parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fileSize</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hearing File Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the file is split into parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fileSize</t>
   </si>
   <si>
     <t xml:space="preserve">Hearing File Size</t>
@@ -1473,7 +1473,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1771,6 +1771,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2413,37 +2417,37 @@
       <c r="X2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="90" t="s">
+      <c r="K3" s="91" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2595,10 +2599,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="62"/>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G4" s="62" t="n">
@@ -2623,10 +2627,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="62"/>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G5" s="62" t="n">
@@ -2651,10 +2655,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="62"/>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F6" s="93" t="s">
+      <c r="F6" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G6" s="62" t="n">
@@ -2679,10 +2683,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="62"/>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="62" t="n">
@@ -2707,10 +2711,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="62"/>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G8" s="62" t="n">
@@ -2735,10 +2739,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="62"/>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="93" t="s">
         <v>227</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="94" t="s">
         <v>228</v>
       </c>
       <c r="G9" s="62" t="n">
@@ -2763,10 +2767,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="62"/>
-      <c r="E10" s="92" t="s">
+      <c r="E10" s="93" t="s">
         <v>229</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="94" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="62" t="n">
@@ -2783,9 +2787,9 @@
       <c r="L10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="H11" s="88"/>
+      <c r="H11" s="89"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2814,184 +2818,184 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="94" width="30.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="94" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="94" width="54.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="94" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="94" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="94" width="44.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="94" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="94" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="94" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="94" width="19.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="94" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="95" width="30.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="95" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="95" width="54.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="95" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="95" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="95" width="44.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="95" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="95" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="95" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="95" width="19.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="95" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="96" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
-      <c r="M1" s="99"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
     </row>
     <row r="2" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="102" t="s">
+      <c r="F2" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="H2" s="104" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="102" t="s">
+      <c r="J2" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="107" t="s">
+      <c r="E3" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="107" t="s">
+      <c r="F3" s="108" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="107" t="s">
+      <c r="G3" s="108" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="108" t="s">
+      <c r="H3" s="109" t="s">
         <v>238</v>
       </c>
-      <c r="I3" s="108" t="s">
+      <c r="I3" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="108" t="s">
+      <c r="J3" s="109" t="s">
         <v>239</v>
       </c>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="109" t="s">
         <v>240</v>
       </c>
-      <c r="L3" s="108"/>
-      <c r="M3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="110"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="111"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
+      <c r="A7" s="111"/>
+      <c r="B7" s="111"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
+      <c r="A8" s="111"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3034,20 +3038,20 @@
       <c r="A1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="114" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3089,10 +3093,10 @@
       <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="116" t="s">
         <v>183</v>
       </c>
       <c r="E3" s="48" t="s">
@@ -3118,7 +3122,7 @@
       <c r="A4" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -3362,46 +3366,46 @@
       <c r="H2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="117" t="s">
+      <c r="I2" s="118" t="s">
         <v>249</v>
       </c>
-      <c r="J2" s="118"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="121" t="s">
+      <c r="I3" s="122" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="122"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="67" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -3513,7 +3517,7 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" s="124" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="125" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
@@ -3536,26 +3540,26 @@
       <c r="J9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="87"/>
+      <c r="A10" s="88"/>
       <c r="C10" s="28"/>
-      <c r="G10" s="125"/>
+      <c r="G10" s="126"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
+      <c r="A11" s="88"/>
       <c r="C11" s="28"/>
-      <c r="G11" s="125"/>
+      <c r="G11" s="126"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="G12" s="125"/>
+      <c r="A12" s="88"/>
+      <c r="G12" s="126"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="G13" s="125"/>
+      <c r="A13" s="88"/>
+      <c r="G13" s="126"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="G14" s="125"/>
+      <c r="A14" s="88"/>
+      <c r="G14" s="126"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3595,7 +3599,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>250</v>
       </c>
       <c r="B1" s="58" t="s">
@@ -3604,60 +3608,60 @@
       <c r="C1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="127" t="s">
+      <c r="D1" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="128" t="s">
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="129" t="s">
         <v>251</v>
       </c>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="128" t="s">
+      <c r="E2" s="129" t="s">
         <v>252</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="90" t="s">
         <v>253</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="130" t="s">
+      <c r="C3" s="131" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="130" t="s">
+      <c r="D3" s="131" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="129" t="s">
+      <c r="E3" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="130" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="130" t="s">
         <v>254</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="130" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3686,35 +3690,35 @@
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="131" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="131" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="132" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="132" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="131" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="131" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="131" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="132" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="132" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="132" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="133" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="135" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3750,34 +3754,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="92" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="91" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3888,7 +3892,7 @@
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
-      <c r="I8" s="136"/>
+      <c r="I8" s="137"/>
       <c r="J8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3910,7 +3914,7 @@
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="136"/>
+      <c r="I9" s="137"/>
       <c r="J9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3932,7 +3936,7 @@
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="136"/>
+      <c r="I10" s="137"/>
       <c r="J10" s="62"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4021,37 +4025,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="120" t="s">
+      <c r="D3" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="90" t="s">
+      <c r="H3" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="91" t="s">
         <v>221</v>
       </c>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="n">
@@ -4208,32 +4212,32 @@
       <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="87"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="F11" s="137"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="138"/>
+      <c r="D11" s="138"/>
+      <c r="F11" s="138"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="87"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="137"/>
-      <c r="F12" s="137"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="F12" s="138"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="137"/>
-      <c r="F13" s="137"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="F13" s="138"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="87"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="F14" s="137"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="F14" s="138"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4315,13 +4319,13 @@
       <c r="C3" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="80" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4330,10 +4334,10 @@
         <v>44197</v>
       </c>
       <c r="B4" s="62"/>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="139" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="138" t="s">
+      <c r="D4" s="139" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="42" t="s">
@@ -4344,8 +4348,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
-      <c r="C5" s="139"/>
+      <c r="A5" s="88"/>
+      <c r="C5" s="140"/>
     </row>
     <row r="6" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4418,31 +4422,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="140" t="s">
+      <c r="D3" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="87"/>
+      <c r="A4" s="88"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="87"/>
+      <c r="A5" s="88"/>
       <c r="C5" s="28"/>
     </row>
   </sheetData>
@@ -4655,7 +4659,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4698,7 +4702,7 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -4715,7 +4719,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="142" t="s">
         <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4727,12 +4731,12 @@
       <c r="D1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="65.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -4753,42 +4757,42 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="145" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="145" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="143" t="s">
+      <c r="F3" s="144" t="s">
         <v>275</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -4815,7 +4819,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -4833,7 +4837,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -4851,7 +4855,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -4869,7 +4873,7 @@
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="116"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
@@ -4887,7 +4891,7 @@
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="116"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
@@ -4905,7 +4909,7 @@
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="116"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
@@ -4923,7 +4927,7 @@
       <c r="A11" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B11" s="116"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
@@ -4941,7 +4945,7 @@
       <c r="A12" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B12" s="116"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="42" t="s">
         <v>38</v>
       </c>
@@ -4959,7 +4963,7 @@
       <c r="A13" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B13" s="116"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="42" t="s">
         <v>38</v>
       </c>
@@ -5081,13 +5085,13 @@
       <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="146" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
       <c r="F3" s="20" t="s">
@@ -5098,7 +5102,7 @@
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="116"/>
+      <c r="B4" s="117"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
@@ -5116,7 +5120,7 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
@@ -5134,7 +5138,7 @@
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="117"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
@@ -5152,7 +5156,7 @@
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
@@ -5198,31 +5202,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="146" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="146" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="146" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="146" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="146" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="146" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="146" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="27.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="255" min="7" style="147" width="14.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="256" style="11" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="148" t="s">
+      <c r="B1" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="149" t="s">
+      <c r="C1" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="150" t="s">
+      <c r="D1" s="151" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -5234,7 +5238,7 @@
       <c r="C2" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="152" t="s">
+      <c r="D2" s="153" t="s">
         <v>283</v>
       </c>
       <c r="E2" s="17" t="s">
@@ -5243,29 +5247,29 @@
       <c r="F2" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="154" t="s">
+      <c r="B3" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="146" t="s">
         <v>284</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="146" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="155" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5319,7 +5323,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5371,10 +5375,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="48" t="s">
@@ -5386,10 +5390,10 @@
       <c r="E3" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="77" t="s">
         <v>221</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="77" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5447,7 +5451,7 @@
         <v>92</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>276</v>
@@ -5481,57 +5485,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="124" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="124" width="41.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="124" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="125" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="125" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="125" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="125" width="41.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="125" width="11.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="157"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="158"/>
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="159" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="158" t="s">
+      <c r="B2" s="159" t="s">
         <v>290</v>
       </c>
-      <c r="C2" s="158" t="s">
+      <c r="C2" s="159" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="158" t="s">
+      <c r="D2" s="159" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="160" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="159" t="s">
+      <c r="B3" s="160" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="C3" s="160" t="s">
         <v>295</v>
       </c>
-      <c r="D3" s="159" t="s">
+      <c r="D3" s="160" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="161" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="162" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="161" t="s">
+      <c r="C4" s="162" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -5539,10 +5543,10 @@
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="162"/>
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="164"/>
+      <c r="A5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="165"/>
     </row>
     <row r="6" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5874,7 +5878,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9447,8 +9451,8 @@
   </sheetPr>
   <dimension ref="A1:IU18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9637,17 +9641,17 @@
       <c r="D5" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="52" t="s">
-        <v>114</v>
+      <c r="E5" s="75" t="s">
+        <v>78</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K5" s="51" t="s">
         <v>41</v>
@@ -9906,10 +9910,10 @@
         <v>95</v>
       </c>
       <c r="D6" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="52" t="s">
         <v>117</v>
-      </c>
-      <c r="E6" s="52" t="s">
-        <v>114</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="52" t="s">
@@ -10179,7 +10183,7 @@
       <c r="E8" s="65"/>
       <c r="F8" s="53"/>
       <c r="G8" s="65"/>
-      <c r="I8" s="75"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="65"/>
@@ -10199,7 +10203,7 @@
       <c r="E11" s="65"/>
       <c r="F11" s="53"/>
       <c r="G11" s="65"/>
-      <c r="I11" s="75"/>
+      <c r="I11" s="76"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="65"/>
@@ -10328,7 +10332,7 @@
       <c r="E3" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="77" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="61"/>
@@ -10344,10 +10348,10 @@
       <c r="C4" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="78" t="s">
         <v>126</v>
       </c>
       <c r="F4" s="62" t="n">
@@ -10362,10 +10366,10 @@
       <c r="C5" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="78" t="s">
         <v>127</v>
       </c>
       <c r="F5" s="62" t="n">
@@ -10439,12 +10443,12 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
       <c r="R1" s="15"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
@@ -10534,10 +10538,10 @@
       <c r="G3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="80" t="s">
         <v>142</v>
       </c>
       <c r="J3" s="20" t="s">
@@ -10564,13 +10568,13 @@
       <c r="R3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="S3" s="76" t="s">
+      <c r="S3" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="76" t="s">
+      <c r="T3" s="77" t="s">
         <v>151</v>
       </c>
-      <c r="U3" s="76" t="s">
+      <c r="U3" s="77" t="s">
         <v>152</v>
       </c>
     </row>
@@ -10607,8 +10611,8 @@
       <c r="N4" s="50"/>
       <c r="O4" s="50"/>
       <c r="P4" s="50"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80" t="s">
+      <c r="R4" s="81"/>
+      <c r="S4" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T4" s="50"/>
@@ -10649,8 +10653,8 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="80" t="s">
+      <c r="R5" s="81"/>
+      <c r="S5" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T5" s="50"/>
@@ -10691,8 +10695,8 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80" t="s">
+      <c r="R6" s="81"/>
+      <c r="S6" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T6" s="50"/>
@@ -10727,20 +10731,20 @@
       <c r="J7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="81"/>
+      <c r="K7" s="82"/>
       <c r="L7" s="50" t="n">
         <v>5</v>
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="82" t="s">
+      <c r="O7" s="83" t="s">
         <v>166</v>
       </c>
       <c r="P7" s="50"/>
-      <c r="R7" s="80" t="s">
+      <c r="R7" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="S7" s="80" t="s">
+      <c r="S7" s="81" t="s">
         <v>156</v>
       </c>
       <c r="T7" s="50"/>
@@ -10946,7 +10950,7 @@
       <c r="O3" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="83" t="s">
+      <c r="P3" s="84" t="s">
         <v>192</v>
       </c>
       <c r="Q3" s="21" t="s">
@@ -10981,7 +10985,7 @@
       <c r="H4" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J4" s="62"/>
@@ -11019,7 +11023,7 @@
       <c r="H5" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J5" s="62"/>
@@ -11059,7 +11063,7 @@
       <c r="H6" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J6" s="62"/>
@@ -11097,7 +11101,7 @@
       <c r="H7" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J7" s="62"/>
@@ -11135,7 +11139,7 @@
       <c r="H8" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="84" t="s">
+      <c r="I8" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J8" s="62"/>
@@ -11173,7 +11177,7 @@
       <c r="H9" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="84" t="s">
+      <c r="I9" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J9" s="62"/>
@@ -11211,7 +11215,7 @@
       <c r="H10" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J10" s="62"/>
@@ -11249,7 +11253,7 @@
       <c r="H11" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J11" s="62"/>
@@ -11287,7 +11291,7 @@
       <c r="H12" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="84" t="s">
+      <c r="I12" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J12" s="62"/>
@@ -11320,12 +11324,12 @@
       <c r="E13" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="H13" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="84" t="s">
+      <c r="I13" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J13" s="62"/>
@@ -11363,7 +11367,7 @@
       <c r="H14" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="84" t="s">
+      <c r="I14" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J14" s="62"/>
@@ -11401,7 +11405,7 @@
       <c r="H15" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="84" t="s">
+      <c r="I15" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J15" s="62"/>
@@ -11439,7 +11443,7 @@
       <c r="H16" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I16" s="84" t="s">
+      <c r="I16" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J16" s="62"/>
@@ -11477,7 +11481,7 @@
       <c r="H17" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="84" t="s">
+      <c r="I17" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J17" s="62"/>
@@ -11515,7 +11519,7 @@
       <c r="H18" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="84" t="s">
+      <c r="I18" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J18" s="62"/>
@@ -11553,7 +11557,7 @@
       <c r="H19" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="84" t="s">
+      <c r="I19" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J19" s="62"/>
@@ -11591,7 +11595,7 @@
       <c r="H20" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="84" t="s">
+      <c r="I20" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J20" s="62"/>
@@ -11629,7 +11633,7 @@
       <c r="H21" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="84" t="s">
+      <c r="I21" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J21" s="62"/>
@@ -11667,7 +11671,7 @@
       <c r="H22" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="84" t="s">
+      <c r="I22" s="85" t="s">
         <v>197</v>
       </c>
       <c r="J22" s="62"/>
@@ -11705,7 +11709,7 @@
       <c r="H23" s="74" t="n">
         <v>1</v>
       </c>
-      <c r="I23" s="86" t="s">
+      <c r="I23" s="87" t="s">
         <v>201</v>
       </c>
       <c r="J23" s="62"/>
@@ -11725,132 +11729,132 @@
       <c r="T23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="87"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="Q24" s="88"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="Q24" s="89"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="88"/>
-      <c r="K25" s="88"/>
-      <c r="L25" s="88"/>
-      <c r="Q25" s="88"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="Q25" s="89"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="Q26" s="88"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="Q26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="87"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="Q27" s="88"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="Q27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="87"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="88"/>
-      <c r="Q28" s="88"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="87"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="88"/>
-      <c r="Q29" s="88"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="Q29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="87"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="Q30" s="88"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="Q30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="87"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="Q31" s="88"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="Q31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="87"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="Q32" s="88"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="Q32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="87"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="89"/>
-      <c r="G33" s="89"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="Q33" s="88"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="Q33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="87"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="Q34" s="88"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="Q34" s="89"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
revert segmentNumber type change
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -417,6 +417,9 @@
     <t xml:space="preserve">segmentNumber</t>
   </si>
   <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hearing File Segment</t>
   </si>
   <si>
@@ -424,9 +427,6 @@
   </si>
   <si>
     <t xml:space="preserve">fileSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
   </si>
   <si>
     <t xml:space="preserve">Hearing File Size</t>
@@ -1043,7 +1043,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1209,6 +1209,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1460,7 +1465,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1774,7 +1779,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1798,7 +1803,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1806,7 +1811,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1922,10 +1927,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1934,15 +1935,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1950,7 +1955,51 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1958,59 +2007,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2018,11 +2015,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2034,7 +2039,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2042,7 +2047,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2122,7 +2127,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2130,11 +2135,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5451,7 +5456,7 @@
         <v>92</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>276</v>
@@ -9452,7 +9457,7 @@
   <dimension ref="A1:IU18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9642,16 +9647,16 @@
         <v>113</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="51" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K5" s="51" t="s">
         <v>41</v>
@@ -9910,10 +9915,10 @@
         <v>95</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="52" t="s">

</xml_diff>

<commit_message>
add xui url to download link for email
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="307">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t xml:space="preserve">Initial case state – create case details as a minimum; add files, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1_CLOSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close the case</t>
   </si>
   <si>
     <t xml:space="preserve">CaseField</t>
@@ -414,19 +423,19 @@
     <t xml:space="preserve">File URL</t>
   </si>
   <si>
-    <t xml:space="preserve">segmentNumber</t>
+    <t xml:space="preserve">segmentNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hearing File Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the file is split into parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fileSize</t>
   </si>
   <si>
     <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hearing File Segment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the file is split into parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fileSize</t>
   </si>
   <si>
     <t xml:space="preserve">Hearing File Size</t>
@@ -593,6 +602,15 @@
   </si>
   <si>
     <t xml:space="preserve">http://172.17.0.1:8080/sharees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closeCase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close a case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close case</t>
   </si>
   <si>
     <t xml:space="preserve">CaseEventToFields</t>
@@ -1043,7 +1061,7 @@
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1209,11 +1227,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1465,7 +1478,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1699,6 +1712,38 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1707,38 +1752,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1776,10 +1789,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1803,7 +1812,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1811,7 +1820,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1927,6 +1940,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1935,7 +1952,27 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1943,15 +1980,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1963,15 +1992,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1979,7 +2004,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1987,27 +2020,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2015,19 +2036,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2039,7 +2052,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2047,7 +2060,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2127,7 +2140,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2135,11 +2148,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="6" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2354,7 +2367,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -2381,31 +2394,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="L2" s="47"/>
       <c r="M2" s="47"/>
@@ -2432,28 +2445,28 @@
         <v>19</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G3" s="91" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H3" s="91" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="I3" s="91" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="J3" s="91" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="K3" s="91" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2497,7 +2510,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="12" t="s">
@@ -2528,31 +2541,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2566,230 +2579,230 @@
         <v>49</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="H3" s="48" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
+        <v>112</v>
+      </c>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F4" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G4" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="62" t="n">
+        <v>74</v>
+      </c>
+      <c r="I4" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="62"/>
+      <c r="J4" s="60"/>
       <c r="K4" s="25"/>
-      <c r="L4" s="62"/>
+      <c r="L4" s="60"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="62"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F5" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G5" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G5" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="62" t="n">
+        <v>78</v>
+      </c>
+      <c r="I5" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F6" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G6" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G6" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H6" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="62" t="n">
+        <v>82</v>
+      </c>
+      <c r="I6" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B7" s="62"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G7" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G7" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="62" t="n">
+        <v>89</v>
+      </c>
+      <c r="I7" s="60" t="n">
         <v>5</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B8" s="62"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F8" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G8" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G8" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="62" t="n">
+        <v>91</v>
+      </c>
+      <c r="I8" s="60" t="n">
         <v>6</v>
       </c>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="62"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="93" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F9" s="94" t="s">
-        <v>228</v>
-      </c>
-      <c r="G9" s="62" t="n">
+        <v>234</v>
+      </c>
+      <c r="G9" s="60" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="62" t="n">
+        <v>93</v>
+      </c>
+      <c r="I9" s="60" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B10" s="62"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="93" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="62" t="n">
+        <v>96</v>
+      </c>
+      <c r="G10" s="60" t="n">
         <v>2</v>
       </c>
       <c r="H10" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" s="62" t="n">
+        <v>95</v>
+      </c>
+      <c r="I10" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="88"/>
@@ -2838,7 +2851,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="96" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B1" s="97" t="s">
         <v>8</v>
@@ -2873,22 +2886,22 @@
         <v>13</v>
       </c>
       <c r="E2" s="103" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F2" s="103" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="G2" s="104" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H2" s="104" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="I2" s="105" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J2" s="103" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="K2" s="104"/>
       <c r="L2" s="106"/>
@@ -2911,22 +2924,22 @@
         <v>50</v>
       </c>
       <c r="F3" s="108" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="G3" s="108" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="H3" s="109" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="I3" s="109" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J3" s="109" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="K3" s="109" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="L3" s="109"/>
       <c r="M3" s="110"/>
@@ -3041,7 +3054,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B1" s="112" t="s">
         <v>8</v>
@@ -3070,25 +3083,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3102,25 +3115,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="116" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3132,11 +3145,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="74" t="n">
@@ -3154,11 +3167,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="52" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5" s="50"/>
       <c r="H5" s="74" t="n">
@@ -3176,11 +3189,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G6" s="50"/>
       <c r="H6" s="74" t="n">
@@ -3198,11 +3211,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="74" t="n">
@@ -3220,11 +3233,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G8" s="50"/>
       <c r="H8" s="74" t="n">
@@ -3237,23 +3250,23 @@
       <c r="A9" s="24" t="n">
         <v>44197</v>
       </c>
-      <c r="B9" s="62"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="62"/>
+        <v>82</v>
+      </c>
+      <c r="E9" s="60"/>
       <c r="F9" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="62"/>
+        <v>83</v>
+      </c>
+      <c r="G9" s="60"/>
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
     </row>
     <row r="10" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="65"/>
@@ -3329,7 +3342,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -3357,22 +3370,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I2" s="118" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="J2" s="119"/>
       <c r="K2" s="120"/>
@@ -3390,22 +3403,22 @@
         <v>49</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="91" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I3" s="122" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="J3" s="123"/>
       <c r="K3" s="124"/>
@@ -3421,11 +3434,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -3443,11 +3456,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="52" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5" s="74" t="n">
         <v>2</v>
@@ -3465,11 +3478,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -3487,11 +3500,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -3509,11 +3522,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G8" s="74" t="n">
         <v>6</v>
@@ -3531,11 +3544,11 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="52" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G9" s="74" t="n">
         <v>7</v>
@@ -3605,12 +3618,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="127" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="57" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="128" t="s">
@@ -3626,16 +3639,16 @@
       <c r="A2" s="90"/>
       <c r="B2" s="90"/>
       <c r="C2" s="129" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D2" s="129" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E2" s="129" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="G2" s="90"/>
       <c r="H2" s="90"/>
@@ -3652,22 +3665,22 @@
         <v>49</v>
       </c>
       <c r="D3" s="131" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="130" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F3" s="130" t="s">
         <v>50</v>
       </c>
       <c r="G3" s="130" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H3" s="130" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="I3" s="130" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3708,7 +3721,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="133" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B1" s="134" t="s">
         <v>8</v>
@@ -3737,25 +3750,25 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3769,25 +3782,25 @@
         <v>49</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G3" s="91" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H3" s="91" t="s">
         <v>50</v>
       </c>
       <c r="I3" s="91" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="J3" s="91" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3799,11 +3812,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="52"/>
       <c r="F4" s="52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="74" t="n">
@@ -3821,11 +3834,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="52"/>
       <c r="F5" s="52" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="74" t="n">
@@ -3843,11 +3856,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="52"/>
       <c r="F6" s="52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="74" t="n">
@@ -3865,11 +3878,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="74" t="n">
@@ -3887,18 +3900,18 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="52" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="74" t="n">
         <v>6</v>
       </c>
       <c r="I8" s="137"/>
-      <c r="J8" s="62"/>
+      <c r="J8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
@@ -3909,18 +3922,18 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="52" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="74" t="n">
         <v>7</v>
       </c>
       <c r="I9" s="137"/>
-      <c r="J9" s="62"/>
+      <c r="J9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="n">
@@ -3931,18 +3944,18 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="74" t="n">
         <v>8</v>
       </c>
       <c r="I10" s="137"/>
-      <c r="J10" s="62"/>
+      <c r="J10" s="60"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3983,7 +3996,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4011,22 +4024,22 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4040,22 +4053,22 @@
         <v>49</v>
       </c>
       <c r="D3" s="121" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G3" s="91" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="91" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I3" s="91" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="J3" s="124"/>
       <c r="K3" s="124"/>
@@ -4071,11 +4084,11 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="52" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G4" s="74" t="n">
         <v>1</v>
@@ -4093,11 +4106,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="52" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G5" s="74" t="n">
         <v>2</v>
@@ -4115,11 +4128,11 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G6" s="74" t="n">
         <v>3</v>
@@ -4137,11 +4150,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G7" s="74" t="n">
         <v>4</v>
@@ -4159,11 +4172,11 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G8" s="74" t="n">
         <v>6</v>
@@ -4181,11 +4194,11 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="52" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G9" s="74" t="n">
         <v>7</v>
@@ -4203,11 +4216,11 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="G10" s="74" t="n">
         <v>8</v>
@@ -4265,7 +4278,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4282,7 +4295,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4305,13 +4318,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4322,25 +4335,25 @@
         <v>18</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>265</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>266</v>
+        <v>269</v>
+      </c>
+      <c r="D3" s="79" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="79" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="139" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D4" s="139" t="s">
         <v>23</v>
@@ -4392,7 +4405,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4414,16 +4427,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4613,7 +4626,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4634,13 +4647,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4654,10 +4667,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4669,10 +4682,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F4" s="53"/>
       <c r="G4" s="53"/>
@@ -4725,7 +4738,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="142" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -4751,16 +4764,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>273</v>
-      </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="G2" s="129"/>
       <c r="H2" s="129"/>
@@ -4779,13 +4792,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="145" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="145" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F3" s="144" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G3" s="90"/>
       <c r="H3" s="90"/>
@@ -4802,13 +4815,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -4829,13 +4842,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4847,13 +4860,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4865,13 +4878,13 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4883,13 +4896,13 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4901,13 +4914,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4919,13 +4932,13 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4937,13 +4950,13 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4955,13 +4968,13 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4973,13 +4986,13 @@
         <v>38</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5044,7 +5057,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5066,16 +5079,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -5094,13 +5107,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E3" s="146" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5112,13 +5125,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5130,13 +5143,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5148,13 +5161,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5165,14 +5178,14 @@
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="62" t="s">
-        <v>163</v>
+      <c r="D7" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F7" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5201,8 +5214,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5219,7 +5232,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="148" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B1" s="149" t="s">
         <v>8</v>
@@ -5241,16 +5254,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D2" s="153" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="G2" s="154"/>
       <c r="H2" s="154"/>
@@ -5269,13 +5282,13 @@
         <v>49</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E3" s="146" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F3" s="155" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5290,10 +5303,10 @@
         <v>52</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -5345,7 +5358,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -5364,42 +5377,42 @@
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="48" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="77" t="s">
-        <v>221</v>
-      </c>
-      <c r="G3" s="77" t="s">
-        <v>275</v>
+        <v>109</v>
+      </c>
+      <c r="F3" s="76" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="4" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5411,16 +5424,16 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5432,16 +5445,16 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5453,16 +5466,16 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="G6" s="51" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -5499,7 +5512,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="156" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B1" s="157"/>
       <c r="C1" s="157"/>
@@ -5507,44 +5520,44 @@
     </row>
     <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="159" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B2" s="159" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C2" s="159" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="D2" s="159" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="160" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="B3" s="160" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C3" s="160" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="D3" s="160" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" s="67" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="161" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B4" s="162" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="C4" s="162" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" s="67" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5734,7 +5747,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5855,9 +5868,36 @@
       <c r="P4" s="53"/>
       <c r="Q4" s="53"/>
     </row>
-    <row r="5" s="54" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="55"/>
-      <c r="C5" s="56"/>
+    <row r="5" s="54" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="49" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B5" s="50"/>
+      <c r="C5" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="50"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5907,16 +5947,16 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="58" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5931,31 +5971,31 @@
         <v>43</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M2" s="47"/>
       <c r="N2" s="47"/>
@@ -5977,34 +6017,34 @@
         <v>19</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
+        <v>73</v>
+      </c>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
@@ -6015,26 +6055,26 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G4" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="62"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
       <c r="AHE4" s="0"/>
       <c r="AHF4" s="0"/>
       <c r="AHG4" s="0"/>
@@ -6180,25 +6220,25 @@
       <c r="C5" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="63" t="s">
-        <v>75</v>
+      <c r="D5" s="61" t="s">
+        <v>78</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
       <c r="AHE5" s="0"/>
       <c r="AHF5" s="0"/>
       <c r="AHG5" s="0"/>
@@ -6344,23 +6384,23 @@
       <c r="C6" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>79</v>
+      <c r="D6" s="61" t="s">
+        <v>82</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
       <c r="J6" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
       <c r="AHE6" s="0"/>
       <c r="AHF6" s="0"/>
       <c r="AHG6" s="0"/>
@@ -6506,25 +6546,25 @@
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
       <c r="AHE7" s="0"/>
       <c r="AHF7" s="0"/>
       <c r="AHG7" s="0"/>
@@ -6670,23 +6710,23 @@
       <c r="C8" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="63" t="s">
-        <v>84</v>
+      <c r="D8" s="61" t="s">
+        <v>87</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="62"/>
+        <v>88</v>
+      </c>
+      <c r="F8" s="60"/>
       <c r="G8" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
       <c r="J8" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
       <c r="AHE8" s="0"/>
       <c r="AHF8" s="0"/>
       <c r="AHG8" s="0"/>
@@ -6832,23 +6872,23 @@
       <c r="C9" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="64" t="s">
-        <v>86</v>
+      <c r="D9" s="62" t="s">
+        <v>89</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="62"/>
+        <v>90</v>
+      </c>
+      <c r="F9" s="60"/>
       <c r="G9" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
       <c r="J9" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
       <c r="AHE9" s="0"/>
       <c r="AHF9" s="0"/>
       <c r="AHG9" s="0"/>
@@ -6994,23 +7034,23 @@
       <c r="C10" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="64" t="s">
-        <v>88</v>
+      <c r="D10" s="62" t="s">
+        <v>91</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="62"/>
+        <v>92</v>
+      </c>
+      <c r="F10" s="60"/>
       <c r="G10" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
       <c r="J10" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
       <c r="AHE10" s="0"/>
       <c r="AHF10" s="0"/>
       <c r="AHG10" s="0"/>
@@ -7156,23 +7196,23 @@
       <c r="C11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="64" t="s">
-        <v>90</v>
+      <c r="D11" s="62" t="s">
+        <v>93</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="62"/>
+        <v>94</v>
+      </c>
+      <c r="F11" s="60"/>
       <c r="G11" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
       <c r="J11" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="AHE11" s="0"/>
       <c r="AHF11" s="0"/>
       <c r="AHG11" s="0"/>
@@ -7319,24 +7359,24 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="51" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" s="62"/>
+        <v>98</v>
+      </c>
+      <c r="I12" s="60"/>
       <c r="J12" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
       <c r="AHE12" s="0"/>
       <c r="AHF12" s="0"/>
       <c r="AHG12" s="0"/>
@@ -7483,22 +7523,22 @@
         <v>38</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="62"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="60"/>
       <c r="G13" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
+        <v>81</v>
+      </c>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
       <c r="J13" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
       <c r="AHE13" s="0"/>
       <c r="AHF13" s="0"/>
       <c r="AHG13" s="0"/>
@@ -7637,8 +7677,8 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="54" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55"/>
-      <c r="C14" s="56"/>
+      <c r="A14" s="63"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="65"/>
       <c r="E14" s="65"/>
       <c r="F14" s="53"/>
@@ -9456,8 +9496,8 @@
   </sheetPr>
   <dimension ref="A1:IU18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9483,7 +9523,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -9514,43 +9554,43 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O2" s="69" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="P2" s="70"/>
       <c r="Q2" s="47"/>
@@ -9567,73 +9607,73 @@
         <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I3" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>37</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>50</v>
       </c>
       <c r="O3" s="72" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="P3" s="73"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
     </row>
     <row r="4" s="54" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="52" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="H4" s="62"/>
+        <v>115</v>
+      </c>
+      <c r="H4" s="60"/>
       <c r="I4" s="74"/>
-      <c r="J4" s="62"/>
+      <c r="J4" s="60"/>
       <c r="K4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" s="54" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="49" t="n">
@@ -9641,22 +9681,22 @@
       </c>
       <c r="B5" s="50"/>
       <c r="C5" s="52" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="75" t="s">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>81</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
+        <v>117</v>
+      </c>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="51" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K5" s="51" t="s">
         <v>41</v>
@@ -9912,22 +9952,22 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="52" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F6" s="50"/>
       <c r="G6" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
+        <v>121</v>
+      </c>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
       <c r="J6" s="52" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="K6" s="51" t="s">
         <v>41</v>
@@ -10188,7 +10228,7 @@
       <c r="E8" s="65"/>
       <c r="F8" s="53"/>
       <c r="G8" s="65"/>
-      <c r="I8" s="76"/>
+      <c r="I8" s="75"/>
     </row>
     <row r="9" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="65"/>
@@ -10208,7 +10248,7 @@
       <c r="E11" s="65"/>
       <c r="F11" s="53"/>
       <c r="G11" s="65"/>
-      <c r="I11" s="76"/>
+      <c r="I11" s="75"/>
     </row>
     <row r="12" s="54" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="65"/>
@@ -10283,7 +10323,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10305,16 +10345,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
@@ -10332,34 +10372,34 @@
         <v>19</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="62" t="n">
+        <v>74</v>
+      </c>
+      <c r="D4" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="60" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10367,17 +10407,17 @@
       <c r="A5" s="49" t="n">
         <v>44197</v>
       </c>
-      <c r="B5" s="62"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="62" t="n">
+        <v>74</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="60" t="n">
         <v>2</v>
       </c>
     </row>
@@ -10398,10 +10438,10 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10431,7 +10471,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10448,12 +10488,12 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
       <c r="R1" s="15"/>
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
@@ -10470,55 +10510,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10543,44 +10583,44 @@
       <c r="G3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="80" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" s="80" t="s">
-        <v>142</v>
+      <c r="H3" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="79" t="s">
+        <v>145</v>
       </c>
       <c r="J3" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="S3" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="T3" s="77" t="s">
-        <v>151</v>
-      </c>
-      <c r="U3" s="77" t="s">
         <v>152</v>
+      </c>
+      <c r="S3" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="T3" s="76" t="s">
+        <v>154</v>
+      </c>
+      <c r="U3" s="76" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10592,13 +10632,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G4" s="50" t="n">
         <v>1</v>
@@ -10616,9 +10656,9 @@
       <c r="N4" s="50"/>
       <c r="O4" s="50"/>
       <c r="P4" s="50"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81" t="s">
-        <v>156</v>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80" t="s">
+        <v>159</v>
       </c>
       <c r="T4" s="50"/>
       <c r="U4" s="50"/>
@@ -10632,13 +10672,13 @@
         <v>38</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G5" s="50" t="n">
         <v>2</v>
@@ -10658,9 +10698,9 @@
       <c r="N5" s="50"/>
       <c r="O5" s="50"/>
       <c r="P5" s="50"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81" t="s">
-        <v>156</v>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80" t="s">
+        <v>159</v>
       </c>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
@@ -10674,13 +10714,13 @@
         <v>38</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F6" s="51" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G6" s="50" t="n">
         <v>3</v>
@@ -10700,9 +10740,9 @@
       <c r="N6" s="50"/>
       <c r="O6" s="50"/>
       <c r="P6" s="50"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81" t="s">
-        <v>156</v>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80" t="s">
+        <v>159</v>
       </c>
       <c r="T6" s="50"/>
       <c r="U6" s="50"/>
@@ -10715,14 +10755,14 @@
       <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="62" t="s">
-        <v>163</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>164</v>
+      <c r="D7" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>167</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G7" s="50" t="n">
         <v>4</v>
@@ -10736,24 +10776,66 @@
       <c r="J7" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="81"/>
       <c r="L7" s="50" t="n">
         <v>5</v>
       </c>
       <c r="M7" s="50"/>
       <c r="N7" s="50"/>
-      <c r="O7" s="83" t="s">
-        <v>166</v>
+      <c r="O7" s="82" t="s">
+        <v>169</v>
       </c>
       <c r="P7" s="50"/>
-      <c r="R7" s="81" t="s">
-        <v>156</v>
-      </c>
-      <c r="S7" s="81" t="s">
-        <v>156</v>
+      <c r="R7" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="S7" s="80" t="s">
+        <v>159</v>
       </c>
       <c r="T7" s="50"/>
       <c r="U7" s="50"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="49" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="50" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10806,7 +10888,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>8</v>
@@ -10845,55 +10927,55 @@
         <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="T2" s="34" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
@@ -10920,55 +11002,55 @@
         <v>49</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="P3" s="84" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="R3" s="21" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10980,10 +11062,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="51"/>
@@ -10991,23 +11073,23 @@
         <v>1</v>
       </c>
       <c r="I4" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J4" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J4" s="60"/>
       <c r="K4" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L4" s="51"/>
-      <c r="M4" s="62" t="n">
+      <c r="M4" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
       <c r="Q4" s="51"/>
       <c r="R4" s="74"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="n">
@@ -11018,10 +11100,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
@@ -11029,23 +11111,23 @@
         <v>1</v>
       </c>
       <c r="I5" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J5" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J5" s="60"/>
       <c r="K5" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L5" s="51"/>
-      <c r="M5" s="62" t="n">
+      <c r="M5" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
       <c r="Q5" s="51"/>
       <c r="R5" s="74"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="24" t="n">
@@ -11056,10 +11138,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="51" t="s">
@@ -11069,23 +11151,23 @@
         <v>1</v>
       </c>
       <c r="I6" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J6" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J6" s="60"/>
       <c r="K6" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L6" s="51"/>
-      <c r="M6" s="62" t="n">
+      <c r="M6" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
       <c r="R6" s="74"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="24" t="n">
@@ -11096,10 +11178,10 @@
         <v>38</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F7" s="51"/>
       <c r="G7" s="51"/>
@@ -11107,23 +11189,23 @@
         <v>1</v>
       </c>
       <c r="I7" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J7" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J7" s="60"/>
       <c r="K7" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L7" s="51"/>
-      <c r="M7" s="62" t="n">
+      <c r="M7" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
       <c r="R7" s="74"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="24" t="n">
@@ -11134,10 +11216,10 @@
         <v>38</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -11145,23 +11227,23 @@
         <v>1</v>
       </c>
       <c r="I8" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J8" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J8" s="60"/>
       <c r="K8" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L8" s="51"/>
-      <c r="M8" s="62" t="n">
+      <c r="M8" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
       <c r="Q8" s="51"/>
       <c r="R8" s="74"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="n">
@@ -11172,10 +11254,10 @@
         <v>38</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
@@ -11183,23 +11265,23 @@
         <v>1</v>
       </c>
       <c r="I9" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J9" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J9" s="60"/>
       <c r="K9" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L9" s="51"/>
-      <c r="M9" s="62" t="n">
+      <c r="M9" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
       <c r="Q9" s="51"/>
       <c r="R9" s="74"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="24" t="n">
@@ -11210,10 +11292,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -11221,23 +11303,23 @@
         <v>1</v>
       </c>
       <c r="I10" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J10" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J10" s="60"/>
       <c r="K10" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L10" s="51"/>
-      <c r="M10" s="62" t="n">
+      <c r="M10" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
       <c r="Q10" s="51"/>
       <c r="R10" s="74"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="n">
@@ -11248,10 +11330,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
@@ -11259,23 +11341,23 @@
         <v>1</v>
       </c>
       <c r="I11" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J11" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J11" s="60"/>
       <c r="K11" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L11" s="51"/>
-      <c r="M11" s="62" t="n">
+      <c r="M11" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
       <c r="Q11" s="51"/>
       <c r="R11" s="74"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="24" t="n">
@@ -11286,10 +11368,10 @@
         <v>38</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
@@ -11297,23 +11379,23 @@
         <v>1</v>
       </c>
       <c r="I12" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J12" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J12" s="60"/>
       <c r="K12" s="74" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="L12" s="51"/>
-      <c r="M12" s="62" t="n">
+      <c r="M12" s="60" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
       <c r="Q12" s="51"/>
       <c r="R12" s="74"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="n">
@@ -11324,10 +11406,10 @@
         <v>38</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F13" s="86"/>
       <c r="G13" s="86"/>
@@ -11335,23 +11417,23 @@
         <v>1</v>
       </c>
       <c r="I13" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J13" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J13" s="60"/>
       <c r="K13" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L13" s="51"/>
-      <c r="M13" s="62" t="n">
+      <c r="M13" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
       <c r="Q13" s="51"/>
       <c r="R13" s="74"/>
-      <c r="S13" s="62"/>
-      <c r="T13" s="62"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="n">
@@ -11362,10 +11444,10 @@
         <v>38</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F14" s="51"/>
       <c r="G14" s="51"/>
@@ -11373,23 +11455,23 @@
         <v>1</v>
       </c>
       <c r="I14" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J14" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J14" s="60"/>
       <c r="K14" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L14" s="51"/>
-      <c r="M14" s="62" t="n">
+      <c r="M14" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N14" s="62"/>
-      <c r="O14" s="62"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
       <c r="R14" s="74"/>
-      <c r="S14" s="62"/>
-      <c r="T14" s="62"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="n">
@@ -11400,10 +11482,10 @@
         <v>38</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
@@ -11411,23 +11493,23 @@
         <v>1</v>
       </c>
       <c r="I15" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J15" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J15" s="60"/>
       <c r="K15" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L15" s="51"/>
-      <c r="M15" s="62" t="n">
+      <c r="M15" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
       <c r="Q15" s="51"/>
       <c r="R15" s="74"/>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="n">
@@ -11438,10 +11520,10 @@
         <v>38</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F16" s="51"/>
       <c r="G16" s="51"/>
@@ -11449,23 +11531,23 @@
         <v>1</v>
       </c>
       <c r="I16" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J16" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J16" s="60"/>
       <c r="K16" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L16" s="51"/>
-      <c r="M16" s="62" t="n">
+      <c r="M16" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
       <c r="Q16" s="51"/>
       <c r="R16" s="74"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="60"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="n">
@@ -11476,10 +11558,10 @@
         <v>38</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
@@ -11487,23 +11569,23 @@
         <v>1</v>
       </c>
       <c r="I17" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J17" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J17" s="60"/>
       <c r="K17" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L17" s="51"/>
-      <c r="M17" s="62" t="n">
+      <c r="M17" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
       <c r="Q17" s="51"/>
       <c r="R17" s="74"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="n">
@@ -11514,10 +11596,10 @@
         <v>38</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -11525,23 +11607,23 @@
         <v>1</v>
       </c>
       <c r="I18" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J18" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J18" s="60"/>
       <c r="K18" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L18" s="51"/>
-      <c r="M18" s="62" t="n">
+      <c r="M18" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N18" s="62"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
       <c r="Q18" s="51"/>
       <c r="R18" s="74"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="n">
@@ -11552,10 +11634,10 @@
         <v>38</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E19" s="52" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
@@ -11563,23 +11645,23 @@
         <v>1</v>
       </c>
       <c r="I19" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J19" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J19" s="60"/>
       <c r="K19" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L19" s="51"/>
-      <c r="M19" s="62" t="n">
+      <c r="M19" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N19" s="62"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
       <c r="Q19" s="51"/>
       <c r="R19" s="74"/>
-      <c r="S19" s="62"/>
-      <c r="T19" s="62"/>
+      <c r="S19" s="60"/>
+      <c r="T19" s="60"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="n">
@@ -11590,10 +11672,10 @@
         <v>38</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -11601,23 +11683,23 @@
         <v>1</v>
       </c>
       <c r="I20" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J20" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J20" s="60"/>
       <c r="K20" s="74" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L20" s="51"/>
-      <c r="M20" s="62" t="n">
+      <c r="M20" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
       <c r="Q20" s="51"/>
       <c r="R20" s="74"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
+      <c r="S20" s="60"/>
+      <c r="T20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="n">
@@ -11628,10 +11710,10 @@
         <v>38</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F21" s="51"/>
       <c r="G21" s="51"/>
@@ -11639,23 +11721,23 @@
         <v>1</v>
       </c>
       <c r="I21" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J21" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J21" s="60"/>
       <c r="K21" s="74" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="L21" s="51"/>
-      <c r="M21" s="62" t="n">
+      <c r="M21" s="60" t="n">
         <v>2</v>
       </c>
-      <c r="N21" s="62"/>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
       <c r="Q21" s="51"/>
       <c r="R21" s="74"/>
-      <c r="S21" s="62"/>
-      <c r="T21" s="62"/>
+      <c r="S21" s="60"/>
+      <c r="T21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="n">
@@ -11666,10 +11748,10 @@
         <v>38</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
@@ -11677,23 +11759,23 @@
         <v>1</v>
       </c>
       <c r="I22" s="85" t="s">
-        <v>197</v>
-      </c>
-      <c r="J22" s="62"/>
+        <v>203</v>
+      </c>
+      <c r="J22" s="60"/>
       <c r="K22" s="74" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="L22" s="51"/>
-      <c r="M22" s="62" t="n">
+      <c r="M22" s="60" t="n">
         <v>3</v>
       </c>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
-      <c r="P22" s="62"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
       <c r="Q22" s="51"/>
       <c r="R22" s="74"/>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="n">
@@ -11703,11 +11785,11 @@
       <c r="C23" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="62" t="s">
-        <v>163</v>
+      <c r="D23" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
@@ -11715,23 +11797,23 @@
         <v>1</v>
       </c>
       <c r="I23" s="87" t="s">
-        <v>201</v>
-      </c>
-      <c r="J23" s="62"/>
+        <v>207</v>
+      </c>
+      <c r="J23" s="60"/>
       <c r="K23" s="25" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="L23" s="51"/>
-      <c r="M23" s="62" t="n">
+      <c r="M23" s="60" t="n">
         <v>4</v>
       </c>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
       <c r="Q23" s="51"/>
       <c r="R23" s="74"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="88"/>

</xml_diff>

<commit_message>
add download response headers
</commit_message>
<xml_diff>
--- a/src/aat/resources/hrs_ccd_case_definition.xlsx
+++ b/src/aat/resources/hrs_ccd_case_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="307">
   <si>
     <t xml:space="preserve">Change History</t>
   </si>
@@ -1824,7 +1824,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5040,7 +5040,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5185,6 +5185,24 @@
         <v>282</v>
       </c>
       <c r="F7" s="51" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="49" t="n">
+        <v>44197</v>
+      </c>
+      <c r="B8" s="117"/>
+      <c r="C8" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>282</v>
+      </c>
+      <c r="F8" s="51" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5214,8 +5232,8 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10440,8 +10458,8 @@
   </sheetPr>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10830,7 +10848,9 @@
       <c r="N8" s="50"/>
       <c r="O8" s="50"/>
       <c r="P8" s="50"/>
-      <c r="R8" s="80"/>
+      <c r="R8" s="80" t="s">
+        <v>159</v>
+      </c>
       <c r="S8" s="80" t="s">
         <v>159</v>
       </c>
@@ -10859,7 +10879,7 @@
   <dimension ref="A1:AG34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>